<commit_message>
Projects now assigned such that no students get the same 1st preference (since enough projects to go around as 1st preference)
However, this is assuming the project's stream distribution 50:50, and student's stream distribution 60:40 is good enough
</commit_message>
<xml_diff>
--- a/Analysis120.xlsx
+++ b/Analysis120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="172">
   <si>
     <t>Research Activity</t>
   </si>
@@ -26,520 +26,508 @@
     <t>Percentage Distribution</t>
   </si>
   <si>
-    <t>writing legal fiction</t>
+    <t>playing rock music</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>0.17%</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies</t>
   </si>
   <si>
     <t>CS+DS</t>
   </si>
   <si>
+    <t>0.25%</t>
+  </si>
+  <si>
+    <t>moaning about men</t>
+  </si>
+  <si>
+    <t>0.42%</t>
+  </si>
+  <si>
+    <t>making action movies</t>
+  </si>
+  <si>
+    <t>writing comedy</t>
+  </si>
+  <si>
+    <t>0.92%</t>
+  </si>
+  <si>
+    <t>running a multinational corporation</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>1.42%</t>
+  </si>
+  <si>
+    <t>singing torch songs</t>
+  </si>
+  <si>
+    <t>promoting greed</t>
+  </si>
+  <si>
+    <t>0.67%</t>
+  </si>
+  <si>
+    <t>handing out flowers</t>
+  </si>
+  <si>
+    <t>1.00%</t>
+  </si>
+  <si>
+    <t>playing basketball</t>
+  </si>
+  <si>
+    <t>0.58%</t>
+  </si>
+  <si>
+    <t>ranting about liberals</t>
+  </si>
+  <si>
+    <t>painting colorful pictures</t>
+  </si>
+  <si>
+    <t>0.50%</t>
+  </si>
+  <si>
+    <t>writing plays</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes</t>
+  </si>
+  <si>
+    <t>promoting liberal values</t>
+  </si>
+  <si>
+    <t>commenting on social issues</t>
+  </si>
+  <si>
+    <t>preparing for war</t>
+  </si>
+  <si>
+    <t>fighting the resistance</t>
+  </si>
+  <si>
+    <t>reporting for The Daily Planet</t>
+  </si>
+  <si>
+    <t>0.83%</t>
+  </si>
+  <si>
+    <t>promoting conservative values</t>
+  </si>
+  <si>
+    <t>0.33%</t>
+  </si>
+  <si>
+    <t>0.08%</t>
+  </si>
+  <si>
+    <t>punching out Nazis</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>studying magic tricks</t>
+  </si>
+  <si>
+    <t>seducing emperors</t>
+  </si>
+  <si>
+    <t>throwing sex parties</t>
+  </si>
+  <si>
+    <t>selling consumer goods</t>
+  </si>
+  <si>
+    <t>seeking revenge</t>
+  </si>
+  <si>
+    <t>inventing electrical marvels</t>
+  </si>
+  <si>
+    <t>lecturing about climate change</t>
+  </si>
+  <si>
+    <t>pioneering new technologies</t>
+  </si>
+  <si>
+    <t>writing about sex</t>
+  </si>
+  <si>
+    <t>watching the sun rise</t>
+  </si>
+  <si>
     <t>0.75%</t>
   </si>
   <si>
-    <t>making new wave movies</t>
-  </si>
-  <si>
-    <t>1.00%</t>
-  </si>
-  <si>
-    <t>testing new technologies</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>partying on yachts</t>
-  </si>
-  <si>
-    <t>0.42%</t>
-  </si>
-  <si>
-    <t>cooking chrystal meth</t>
+    <t>writing TV comedies</t>
+  </si>
+  <si>
+    <t>promoting Eastern philosophy</t>
+  </si>
+  <si>
+    <t>composing classical music</t>
+  </si>
+  <si>
+    <t>promoting hair products</t>
+  </si>
+  <si>
+    <t>fighting for the rebel alliance</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
+  </si>
+  <si>
+    <t>testing scientific theories</t>
+  </si>
+  <si>
+    <t>chasing starlets</t>
+  </si>
+  <si>
+    <t>defending plaintiffs</t>
+  </si>
+  <si>
+    <t>playing soccer</t>
+  </si>
+  <si>
+    <t>designing clothes</t>
+  </si>
+  <si>
+    <t>carrying secret plans</t>
+  </si>
+  <si>
+    <t>starring in action movies</t>
+  </si>
+  <si>
+    <t>working for the forces of darkness</t>
+  </si>
+  <si>
+    <t>insulting minorities</t>
+  </si>
+  <si>
+    <t>killing people in ingenious ways</t>
+  </si>
+  <si>
+    <t>chasing criminals</t>
+  </si>
+  <si>
+    <t>1.08%</t>
+  </si>
+  <si>
+    <t>counting tooth picks</t>
+  </si>
+  <si>
+    <t>solving mysteries</t>
   </si>
   <si>
     <t>1.33%</t>
   </si>
   <si>
-    <t>promoting conservative values</t>
-  </si>
-  <si>
-    <t>0.67%</t>
-  </si>
-  <si>
-    <t>singing pop songs</t>
-  </si>
-  <si>
-    <t>0.08%</t>
-  </si>
-  <si>
-    <t>embezzling tax money</t>
-  </si>
-  <si>
-    <t>0.83%</t>
-  </si>
-  <si>
-    <t>running for the presidency</t>
-  </si>
-  <si>
-    <t>0.33%</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
-    <t>stabbing in the back</t>
-  </si>
-  <si>
-    <t>striving for world domination</t>
-  </si>
-  <si>
-    <t>0.50%</t>
+    <t>fighting for civil rights</t>
+  </si>
+  <si>
+    <t>singing to teenagers</t>
+  </si>
+  <si>
+    <t>piloting the Millenium Falcon</t>
+  </si>
+  <si>
+    <t>offering advice</t>
+  </si>
+  <si>
+    <t>finding clues</t>
+  </si>
+  <si>
+    <t>leading revolts</t>
+  </si>
+  <si>
+    <t>1.25%</t>
+  </si>
+  <si>
+    <t>writing modern fiction</t>
+  </si>
+  <si>
+    <t>developing new technologies</t>
+  </si>
+  <si>
+    <t>flying into a rage</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
+  </si>
+  <si>
+    <t>running a business empire</t>
+  </si>
+  <si>
+    <t>making dumb comedies</t>
+  </si>
+  <si>
+    <t>writing about manly pursuits</t>
+  </si>
+  <si>
+    <t>running an empire</t>
+  </si>
+  <si>
+    <t>bodybuilding</t>
+  </si>
+  <si>
+    <t>representing criminals</t>
+  </si>
+  <si>
+    <t>smuggling contraband</t>
+  </si>
+  <si>
+    <t>1.17%</t>
+  </si>
+  <si>
+    <t>singing experimental songs</t>
+  </si>
+  <si>
+    <t>exploring foreign countries</t>
+  </si>
+  <si>
+    <t>doing stand-up</t>
+  </si>
+  <si>
+    <t>robbing banks</t>
+  </si>
+  <si>
+    <t>starring in reality TV shows</t>
+  </si>
+  <si>
+    <t>campaigning for world peace</t>
   </si>
   <si>
     <t>recording pop songs</t>
   </si>
   <si>
-    <t>building giant walls</t>
+    <t>writing short stories</t>
+  </si>
+  <si>
+    <t>promoting communism</t>
+  </si>
+  <si>
+    <t>recruiting dissidents</t>
+  </si>
+  <si>
+    <t>peacocking in fancy clothes</t>
+  </si>
+  <si>
+    <t>opening new markets</t>
+  </si>
+  <si>
+    <t>driving under the influence</t>
+  </si>
+  <si>
+    <t>building houses for poor people</t>
+  </si>
+  <si>
+    <t>making trains run on time</t>
+  </si>
+  <si>
+    <t>developing operating systems</t>
+  </si>
+  <si>
+    <t>performing physical therapy</t>
+  </si>
+  <si>
+    <t>pulling dirty political tricks</t>
+  </si>
+  <si>
+    <t>pedalling furiously</t>
+  </si>
+  <si>
+    <t>singing rock songs</t>
+  </si>
+  <si>
+    <t>frying crabby patties</t>
+  </si>
+  <si>
+    <t>promoting Fascism</t>
+  </si>
+  <si>
+    <t>looking for love</t>
+  </si>
+  <si>
+    <t>developing advertising campaigns</t>
+  </si>
+  <si>
+    <t>writing plays about the middle classes</t>
+  </si>
+  <si>
+    <t>eluding electronic ghosts</t>
+  </si>
+  <si>
+    <t>spouting movie trivia</t>
+  </si>
+  <si>
+    <t>studying science</t>
+  </si>
+  <si>
+    <t>preaching to presidents</t>
+  </si>
+  <si>
+    <t>promoting logical thinking</t>
+  </si>
+  <si>
+    <t>plotting election strategies</t>
+  </si>
+  <si>
+    <t>convicting criminals</t>
+  </si>
+  <si>
+    <t>promoting air travel</t>
+  </si>
+  <si>
+    <t>complaining about everything</t>
+  </si>
+  <si>
+    <t>assassinating presidents</t>
+  </si>
+  <si>
+    <t>preventing terrorism</t>
+  </si>
+  <si>
+    <t>podcasting about movies</t>
+  </si>
+  <si>
+    <t>running a technology company</t>
+  </si>
+  <si>
+    <t>writing in ledgers</t>
+  </si>
+  <si>
+    <t>suppressing violent urges</t>
+  </si>
+  <si>
+    <t>running a media empire</t>
   </si>
   <si>
     <t>promoting capitalism</t>
   </si>
   <si>
-    <t>pioneering new technologies</t>
-  </si>
-  <si>
-    <t>playing rock guitar</t>
-  </si>
-  <si>
-    <t>0.25%</t>
-  </si>
-  <si>
-    <t>clipping coupons</t>
-  </si>
-  <si>
-    <t>writing pot-boilers</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies</t>
-  </si>
-  <si>
-    <t>0.92%</t>
+    <t>foiling the schemes of evil villains</t>
+  </si>
+  <si>
+    <t>wielding political power</t>
+  </si>
+  <si>
+    <t>teaching philosophy</t>
+  </si>
+  <si>
+    <t>painting realistic pictures</t>
+  </si>
+  <si>
+    <t>escaping from water tanks</t>
+  </si>
+  <si>
+    <t>avoiding paparazzi</t>
+  </si>
+  <si>
+    <t>preventing crime</t>
+  </si>
+  <si>
+    <t>chasing flappers</t>
+  </si>
+  <si>
+    <t>drawing whimsical cartoons</t>
+  </si>
+  <si>
+    <t>playing tough guys</t>
+  </si>
+  <si>
+    <t>writing mystery stories</t>
+  </si>
+  <si>
+    <t>smoking herb</t>
+  </si>
+  <si>
+    <t>moaning about women</t>
+  </si>
+  <si>
+    <t>killing murderers</t>
+  </si>
+  <si>
+    <t>singing country music</t>
+  </si>
+  <si>
+    <t>running a large metropolitan city</t>
+  </si>
+  <si>
+    <t>climbing social ladders</t>
   </si>
   <si>
     <t>developing military strategies</t>
   </si>
   <si>
-    <t>0.58%</t>
-  </si>
-  <si>
-    <t>signing sports memorabilia</t>
-  </si>
-  <si>
-    <t>running the FBI</t>
-  </si>
-  <si>
-    <t>promoting Eastern philosophy</t>
-  </si>
-  <si>
-    <t>playing tough guys</t>
-  </si>
-  <si>
-    <t>making topiary sculptures</t>
-  </si>
-  <si>
-    <t>1.08%</t>
-  </si>
-  <si>
-    <t>spreading revolution</t>
+    <t>fighting with swords</t>
+  </si>
+  <si>
+    <t>singing melancholy songs</t>
+  </si>
+  <si>
+    <t>running a criminal empire</t>
+  </si>
+  <si>
+    <t>building rocket ships</t>
+  </si>
+  <si>
+    <t>winning Michelin stars</t>
+  </si>
+  <si>
+    <t>writing poetry</t>
+  </si>
+  <si>
+    <t>instigating rebellion</t>
+  </si>
+  <si>
+    <t>inventing new technologies</t>
+  </si>
+  <si>
+    <t>racking up marriages</t>
+  </si>
+  <si>
+    <t>painting dark pictures</t>
+  </si>
+  <si>
+    <t>following the money</t>
+  </si>
+  <si>
+    <t>falling gracefully</t>
   </si>
   <si>
     <t>offering medical opinions</t>
   </si>
   <si>
-    <t>starring in indy movies</t>
-  </si>
-  <si>
-    <t>peacocking in fancy clothes</t>
-  </si>
-  <si>
-    <t>writing pop songs</t>
-  </si>
-  <si>
-    <t>eluding capture</t>
-  </si>
-  <si>
-    <t>writing blues songs</t>
-  </si>
-  <si>
-    <t>writing sonnets</t>
-  </si>
-  <si>
-    <t>0.17%</t>
+    <t>leaking classified documents</t>
   </si>
   <si>
     <t>making fantasy movies</t>
   </si>
   <si>
-    <t>directing weird movies</t>
-  </si>
-  <si>
-    <t>smoking Boyard cigarettes</t>
-  </si>
-  <si>
-    <t>enjoying ball-room dancing</t>
-  </si>
-  <si>
-    <t>exploring foreign countries</t>
-  </si>
-  <si>
-    <t>singing Hipbop songs</t>
-  </si>
-  <si>
-    <t>promoting feminism</t>
-  </si>
-  <si>
-    <t>knocking out opponents</t>
-  </si>
-  <si>
-    <t>running a budget airline</t>
-  </si>
-  <si>
-    <t>writing crime stories</t>
-  </si>
-  <si>
-    <t>campaigning for social causes</t>
-  </si>
-  <si>
-    <t>writing historical fiction</t>
-  </si>
-  <si>
-    <t>doing stand-up</t>
-  </si>
-  <si>
-    <t>making ice sculptures</t>
-  </si>
-  <si>
-    <t>providing comic relief</t>
-  </si>
-  <si>
-    <t>bullying neighboring countries</t>
-  </si>
-  <si>
-    <t>hunting wabbits</t>
-  </si>
-  <si>
-    <t>writing poetry</t>
-  </si>
-  <si>
-    <t>pulling capers</t>
-  </si>
-  <si>
-    <t>delivering judgments</t>
-  </si>
-  <si>
-    <t>nurturing sibling rivalry</t>
-  </si>
-  <si>
-    <t>solving crimes</t>
-  </si>
-  <si>
-    <t>developing new technologies</t>
-  </si>
-  <si>
-    <t>working in a freak show</t>
-  </si>
-  <si>
-    <t>abusing power</t>
-  </si>
-  <si>
-    <t>creating an axis of evil</t>
-  </si>
-  <si>
-    <t>promoting monetarism</t>
-  </si>
-  <si>
-    <t>making money</t>
-  </si>
-  <si>
-    <t>singing melancholy songs</t>
-  </si>
-  <si>
-    <t>playing rock piano</t>
-  </si>
-  <si>
-    <t>1.25%</t>
-  </si>
-  <si>
-    <t>guarding the galaxy</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>studying symbols</t>
-  </si>
-  <si>
-    <t>singing torch songs</t>
-  </si>
-  <si>
-    <t>singing reggae songs</t>
-  </si>
-  <si>
-    <t>offering advice</t>
-  </si>
-  <si>
-    <t>running a clandestine spy organization</t>
-  </si>
-  <si>
-    <t>waiting for a hero</t>
-  </si>
-  <si>
-    <t>composing classical music</t>
-  </si>
-  <si>
-    <t>making movies</t>
-  </si>
-  <si>
-    <t>promoting big business</t>
-  </si>
-  <si>
-    <t>promoting liberal values</t>
-  </si>
-  <si>
-    <t>promoting science</t>
-  </si>
-  <si>
-    <t>foiling the schemes of evil villains</t>
-  </si>
-  <si>
-    <t>running gentleman's clubs</t>
-  </si>
-  <si>
-    <t>making sarcastic remarks</t>
-  </si>
-  <si>
-    <t>winning heavyweight titles</t>
-  </si>
-  <si>
-    <t>counting cards</t>
-  </si>
-  <si>
-    <t>writing rock songs</t>
-  </si>
-  <si>
-    <t>stealing jewels</t>
-  </si>
-  <si>
-    <t>hosting reality TV shows</t>
-  </si>
-  <si>
-    <t>inventing electrical marvels</t>
-  </si>
-  <si>
-    <t>building replicants</t>
-  </si>
-  <si>
-    <t>getting plastic surgery</t>
-  </si>
-  <si>
-    <t>starring in pornographic movies</t>
-  </si>
-  <si>
-    <t>using gadgets</t>
-  </si>
-  <si>
-    <t>cooking for friends</t>
-  </si>
-  <si>
-    <t>drinking tea</t>
-  </si>
-  <si>
-    <t>making unauthorized sex tapes</t>
-  </si>
-  <si>
-    <t>telling affable jokes</t>
-  </si>
-  <si>
-    <t>recording history</t>
-  </si>
-  <si>
-    <t>disappointing suitors</t>
-  </si>
-  <si>
-    <t>hosting radio shows</t>
-  </si>
-  <si>
-    <t>racking up marriages</t>
-  </si>
-  <si>
-    <t>grabbing power</t>
-  </si>
-  <si>
-    <t>selling tat</t>
-  </si>
-  <si>
-    <t>talking up the economy</t>
-  </si>
-  <si>
-    <t>starring in sit-coms</t>
-  </si>
-  <si>
-    <t>over-achieving at school</t>
-  </si>
-  <si>
-    <t>1.17%</t>
-  </si>
-  <si>
-    <t>running a hardware company</t>
-  </si>
-  <si>
-    <t>issuing threats</t>
-  </si>
-  <si>
     <t>investigating alien abductions</t>
   </si>
   <si>
-    <t>piquing public interest</t>
-  </si>
-  <si>
-    <t>moaning about men</t>
-  </si>
-  <si>
-    <t>playing God</t>
-  </si>
-  <si>
-    <t>reporting for The Daily Planet</t>
-  </si>
-  <si>
-    <t>writing about social problems</t>
-  </si>
-  <si>
-    <t>monetizing celebrity status</t>
-  </si>
-  <si>
-    <t>1.58%</t>
-  </si>
-  <si>
-    <t>running a kingdom</t>
-  </si>
-  <si>
-    <t>working out</t>
-  </si>
-  <si>
-    <t>practicing insincerity</t>
-  </si>
-  <si>
-    <t>doing the Charleston</t>
-  </si>
-  <si>
-    <t>starring in action movies</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes</t>
-  </si>
-  <si>
-    <t>rescuing kids</t>
-  </si>
-  <si>
-    <t>playing grungy music</t>
-  </si>
-  <si>
-    <t>arguing against capitalism</t>
-  </si>
-  <si>
-    <t>hacking into corporate mainframes</t>
-  </si>
-  <si>
-    <t>being condescending to customers</t>
-  </si>
-  <si>
-    <t>living amongst apes</t>
-  </si>
-  <si>
-    <t>avoiding eye contact</t>
-  </si>
-  <si>
-    <t>wielding political power</t>
-  </si>
-  <si>
-    <t>cooking dinners</t>
-  </si>
-  <si>
-    <t>singing protest songs</t>
-  </si>
-  <si>
-    <t>popping amphetamines</t>
-  </si>
-  <si>
-    <t>writing political satires</t>
-  </si>
-  <si>
-    <t>trimming bushes</t>
-  </si>
-  <si>
-    <t>promoting Catholic values</t>
-  </si>
-  <si>
-    <t>writing cook books</t>
-  </si>
-  <si>
-    <t>forming new social connections</t>
-  </si>
-  <si>
-    <t>making racist jibes</t>
-  </si>
-  <si>
-    <t>coining sparkling witticisms</t>
-  </si>
-  <si>
-    <t>1.50%</t>
-  </si>
-  <si>
-    <t>winning tennis matches</t>
-  </si>
-  <si>
-    <t>blowing smoke rings</t>
-  </si>
-  <si>
-    <t>eating donuts</t>
-  </si>
-  <si>
-    <t>playing aggressive chess</t>
-  </si>
-  <si>
-    <t>spitting while speaking</t>
-  </si>
-  <si>
-    <t>gurning for the camera</t>
-  </si>
-  <si>
-    <t>playing basketball</t>
-  </si>
-  <si>
-    <t>chasing after women</t>
-  </si>
-  <si>
-    <t>spreading political gossip</t>
-  </si>
-  <si>
-    <t>campaigning for world peace</t>
-  </si>
-  <si>
-    <t>proving math theorems</t>
-  </si>
-  <si>
-    <t>playing rock music</t>
-  </si>
-  <si>
-    <t>running a tech giant</t>
-  </si>
-  <si>
-    <t>spouting movie trivia</t>
-  </si>
-  <si>
-    <t>recruiting dissidents</t>
+    <t>making escape plans</t>
+  </si>
+  <si>
+    <t>being a good neighbor</t>
+  </si>
+  <si>
+    <t>duelling acrobatically</t>
+  </si>
+  <si>
+    <t>building a search engine</t>
   </si>
 </sst>
 </file>
@@ -597,7 +585,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="35.4296875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="34.9609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.69921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.85546875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="28.9375" customWidth="true" bestFit="true"/>
@@ -625,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3809221946513302</v>
+        <v>0.12365953745407593</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -636,41 +624,41 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>0.38510139543978944</v>
+        <v>0.3081660877607913</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2773682725812654</v>
+        <v>0.36716977630315917</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.36128551897012023</v>
+        <v>0.17221262028805595</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -678,10 +666,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3955523360781059</v>
+        <v>0.2655117594509621</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -692,27 +680,27 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3935677499593202</v>
+        <v>0.38845540188193356</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>0.04251830807419484</v>
+        <v>0.03288585961340481</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -720,10 +708,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3683767111980379</v>
+        <v>0.24978323433855135</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -734,10 +722,10 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1604902900550165</v>
+        <v>0.3086112101385406</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -745,13 +733,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03660802371234025</v>
+        <v>0.3461643239938675</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -762,13 +750,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>0.39420673054065963</v>
+        <v>0.39132421848624854</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -776,10 +764,10 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3253743960454693</v>
+        <v>0.25481152457306144</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -793,10 +781,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>0.14006843552189235</v>
+        <v>0.30897974719167964</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
@@ -804,13 +792,13 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3977421467670922</v>
+        <v>0.38259560949729304</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
@@ -821,10 +809,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.35547582265629446</v>
+        <v>0.3901038070756383</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -832,13 +820,13 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3941386238837456</v>
+        <v>0.35457822594702904</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
@@ -846,41 +834,41 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>0.06042685592420508</v>
+        <v>0.27788817386895714</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C19" t="n">
-        <v>0.15969458593236785</v>
+        <v>0.35352196312379774</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.27811472405602516</v>
+      </c>
+      <c r="D20" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.3964371520345163</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -888,94 +876,94 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C21" t="n">
-        <v>0.36737441088620026</v>
+        <v>0.2887532183039643</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>0.29235743773580847</v>
+        <v>0.12766579764148503</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.18901450615782994</v>
+        <v>0.39015153967339955</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.33372385655261394</v>
+        <v>0.3892826310584495</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.01516138471618333</v>
+      </c>
+      <c r="D25" t="s">
         <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.3849713139787381</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2769355482936898</v>
+        <v>0.38994686380694266</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C27" t="n">
-        <v>0.26876891812500264</v>
+        <v>0.10526104554650073</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -983,30 +971,30 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C28" t="n">
-        <v>0.3240513607766667</v>
+        <v>0.26093907813436523</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C29" t="n">
-        <v>0.37397225978804266</v>
+        <v>0.18584677865155758</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
@@ -1014,55 +1002,55 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3165797956576732</v>
+        <v>0.3981158216832802</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C31" t="n">
-        <v>0.22553219329661886</v>
+        <v>0.2949012128340598</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3792597008570295</v>
+        <v>0.25259837387002093</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C33" t="n">
-        <v>0.27707723584220234</v>
+        <v>0.37677821407813844</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
@@ -1070,55 +1058,55 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>0.39772779270965813</v>
+        <v>0.23324768784803546</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C35" t="n">
-        <v>0.39892854379897086</v>
+        <v>0.3067249494379602</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C36" t="n">
-        <v>0.3509067307455187</v>
+        <v>0.3400192858795854</v>
       </c>
       <c r="D36" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.1969789147883943</v>
+      </c>
+      <c r="D37" t="s">
         <v>51</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0.3572235734725415</v>
-      </c>
-      <c r="D37" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38">
@@ -1126,13 +1114,13 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C38" t="n">
-        <v>0.06187969510711136</v>
+        <v>0.2364629732325973</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
@@ -1140,97 +1128,97 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C39" t="n">
-        <v>0.19368609536136577</v>
+        <v>0.1963999777565019</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>0.33617010606275516</v>
+        <v>0.11671925738023523</v>
       </c>
       <c r="D40" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C41" t="n">
-        <v>0.39154830313718253</v>
+        <v>0.36071431386035857</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C42" t="n">
-        <v>0.39092675843057195</v>
+        <v>0.3224424896438208</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>0.21904451962832264</v>
+        <v>0.19933285509828066</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>0.3534981157647179</v>
+        <v>0.08083283693597261</v>
       </c>
       <c r="D44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2020201197057528</v>
+        <v>0.34903379663558254</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46">
@@ -1238,10 +1226,10 @@
         <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C46" t="n">
-        <v>0.34035910691932514</v>
+        <v>0.3989139469669982</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
@@ -1252,13 +1240,13 @@
         <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.288064594768427</v>
+        <v>0.18810862037542894</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
@@ -1266,13 +1254,13 @@
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C48" t="n">
-        <v>0.05503506508282964</v>
+        <v>0.347740007437327</v>
       </c>
       <c r="D48" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49">
@@ -1280,13 +1268,13 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C49" t="n">
-        <v>0.39683758088370596</v>
+        <v>0.3921122762843404</v>
       </c>
       <c r="D49" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -1294,83 +1282,83 @@
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C50" t="n">
-        <v>0.3492925432877145</v>
+        <v>0.24421794261879945</v>
       </c>
       <c r="D50" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>0.3346995427209048</v>
+        <v>0.36509615466475986</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C52" t="n">
-        <v>0.28277191512159366</v>
+        <v>0.13912601209466585</v>
       </c>
       <c r="D52" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>0.10826214878016048</v>
+        <v>0.152706692845559</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2620092345849021</v>
+        <v>0.3939916535312771</v>
       </c>
       <c r="D54" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.2748630531424906</v>
+      </c>
+      <c r="D55" t="s">
         <v>69</v>
-      </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.33605729511223276</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -1378,27 +1366,27 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C56" t="n">
-        <v>0.38095358615474983</v>
+        <v>0.39876792017613866</v>
       </c>
       <c r="D56" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C57" t="n">
-        <v>0.23778109465132766</v>
+        <v>0.3663865152402292</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58">
@@ -1406,69 +1394,69 @@
         <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C58" t="n">
-        <v>0.2898999601644785</v>
+        <v>0.3986635675595113</v>
       </c>
       <c r="D58" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C59" t="n">
-        <v>0.33709710276657906</v>
+        <v>0.20571368375477841</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C60" t="n">
-        <v>0.006133557283755384</v>
+        <v>0.3548975411742942</v>
       </c>
       <c r="D60" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C61" t="n">
-        <v>0.15631040771447285</v>
+        <v>0.07476486079881246</v>
       </c>
       <c r="D61" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C62" t="n">
-        <v>0.2448711006983925</v>
+        <v>0.3520112472582488</v>
       </c>
       <c r="D62" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63">
@@ -1476,290 +1464,290 @@
         <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C63" t="n">
-        <v>0.024193610804074846</v>
+        <v>0.3517973635248737</v>
       </c>
       <c r="D63" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C64" t="n">
-        <v>0.3031842529493901</v>
+        <v>0.07993519948598601</v>
       </c>
       <c r="D64" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C65" t="n">
-        <v>0.12059170821981094</v>
+        <v>0.3962334563097132</v>
       </c>
       <c r="D65" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C66" t="n">
-        <v>0.06373008178497078</v>
+        <v>0.39316243326708006</v>
       </c>
       <c r="D66" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C67" t="n">
-        <v>0.2634600446405472</v>
+        <v>0.2485267459194358</v>
       </c>
       <c r="D67" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C68" t="n">
-        <v>0.35548488652513943</v>
+        <v>0.17937095351282456</v>
       </c>
       <c r="D68" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C69" t="n">
-        <v>0.33909373264366005</v>
+        <v>0.003170425617031888</v>
       </c>
       <c r="D69" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C70" t="n">
-        <v>0.09129942125699238</v>
+        <v>0.13268138930978596</v>
       </c>
       <c r="D70" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1045672181863037</v>
+        <v>0.3980529481707508</v>
       </c>
       <c r="D71" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C72" t="n">
-        <v>0.3597413594981905</v>
+        <v>0.3380708317513376</v>
       </c>
       <c r="D72" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C73" t="n">
-        <v>0.021687254860696118</v>
+        <v>0.27693515359107357</v>
       </c>
       <c r="D73" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C74" t="n">
-        <v>0.3880834951770229</v>
+        <v>0.07046566766835163</v>
       </c>
       <c r="D74" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C75" t="n">
-        <v>0.2140304236153385</v>
+        <v>0.39838279261407145</v>
       </c>
       <c r="D75" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C76" t="n">
-        <v>0.01382695428127588</v>
+        <v>0.2660149345362879</v>
       </c>
       <c r="D76" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1959218748409784</v>
+        <v>0.05861664668347628</v>
       </c>
       <c r="D77" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C78" t="n">
-        <v>0.012926318406922188</v>
+        <v>0.12755064387338266</v>
       </c>
       <c r="D78" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C79" t="n">
-        <v>0.3185754962375079</v>
+        <v>0.39883739011868574</v>
       </c>
       <c r="D79" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" t="n">
-        <v>0.10483221396509419</v>
+        <v>0.38120672526689475</v>
       </c>
       <c r="D80" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2318673755450568</v>
+        <v>0.34338774094644026</v>
       </c>
       <c r="D81" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C82" t="n">
-        <v>0.10536250417141294</v>
+        <v>0.21774113798309477</v>
       </c>
       <c r="D82" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3988950736318885</v>
+        <v>0.3519214270761913</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
@@ -1767,44 +1755,44 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C84" t="n">
-        <v>0.2396302469641715</v>
+        <v>0.04863864293838953</v>
       </c>
       <c r="D84" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C85" t="n">
-        <v>0.2824982282348297</v>
+        <v>0.3890763265647619</v>
       </c>
       <c r="D85" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
       <c r="C86" t="n">
-        <v>0.39397762589619506</v>
+        <v>0.3786112961307445</v>
       </c>
       <c r="D86" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87">
@@ -1812,13 +1800,13 @@
         <v>99</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C87" t="n">
-        <v>0.12419645487862357</v>
+        <v>0.3123177750385231</v>
       </c>
       <c r="D87" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88">
@@ -1829,10 +1817,10 @@
         <v>5</v>
       </c>
       <c r="C88" t="n">
-        <v>0.3935438454449288</v>
+        <v>0.3529212435730347</v>
       </c>
       <c r="D88" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89">
@@ -1840,13 +1828,13 @@
         <v>101</v>
       </c>
       <c r="B89" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C89" t="n">
-        <v>0.09355020060521603</v>
+        <v>0.09227333916875784</v>
       </c>
       <c r="D89" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90">
@@ -1857,10 +1845,10 @@
         <v>5</v>
       </c>
       <c r="C90" t="n">
-        <v>0.17898499632517612</v>
+        <v>0.3985993715745561</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="91">
@@ -1868,13 +1856,13 @@
         <v>103</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C91" t="n">
-        <v>0.19287134900232378</v>
+        <v>0.39747431251602994</v>
       </c>
       <c r="D91" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92">
@@ -1882,13 +1870,13 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C92" t="n">
-        <v>0.33127782939470346</v>
+        <v>0.2648311974789042</v>
       </c>
       <c r="D92" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93">
@@ -1896,97 +1884,97 @@
         <v>105</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C93" t="n">
-        <v>0.2479003489972061</v>
+        <v>0.3579013315330324</v>
       </c>
       <c r="D93" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C94" t="n">
-        <v>0.14461704824361596</v>
+        <v>0.3034873180936606</v>
       </c>
       <c r="D94" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95" t="n">
-        <v>0.281463301670658</v>
+        <v>0.36699602062983994</v>
       </c>
       <c r="D95" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C96" t="n">
-        <v>0.33478024299246667</v>
+        <v>0.25897535143439976</v>
       </c>
       <c r="D96" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C97" t="n">
-        <v>0.22030971041320863</v>
+        <v>0.39890444248500023</v>
       </c>
       <c r="D97" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C98" t="n">
-        <v>0.394718381170614</v>
+        <v>0.09011786084235188</v>
       </c>
       <c r="D98" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C99" t="n">
-        <v>0.34976479175117453</v>
+        <v>0.38733628824757993</v>
       </c>
       <c r="D99" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100">
@@ -1994,27 +1982,27 @@
         <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C100" t="n">
-        <v>0.11639714832897025</v>
+        <v>0.36507778600493346</v>
       </c>
       <c r="D100" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C101" t="n">
-        <v>0.34705592474819763</v>
+        <v>0.29981050018305444</v>
       </c>
       <c r="D101" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102">
@@ -2022,13 +2010,13 @@
         <v>111</v>
       </c>
       <c r="B102" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C102" t="n">
-        <v>0.31314847922440675</v>
+        <v>0.30427328177379676</v>
       </c>
       <c r="D102" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103">
@@ -2036,10 +2024,10 @@
         <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C103" t="n">
-        <v>0.32985345443431113</v>
+        <v>0.16128021956448022</v>
       </c>
       <c r="D103" t="s">
         <v>20</v>
@@ -2050,13 +2038,13 @@
         <v>113</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C104" t="n">
-        <v>0.23370822755761644</v>
+        <v>0.37084387925311324</v>
       </c>
       <c r="D104" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105">
@@ -2064,153 +2052,153 @@
         <v>114</v>
       </c>
       <c r="B105" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C105" t="n">
-        <v>0.39848309257619474</v>
+        <v>0.3640868339126881</v>
       </c>
       <c r="D105" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C106" t="n">
-        <v>0.3175305912095667</v>
+        <v>0.26916621081657593</v>
       </c>
       <c r="D106" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B107" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C107" t="n">
-        <v>0.37237324123171045</v>
+        <v>0.395038162282362</v>
       </c>
       <c r="D107" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B108" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C108" t="n">
-        <v>0.11853873303273874</v>
+        <v>0.22324043306376562</v>
       </c>
       <c r="D108" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C109" t="n">
-        <v>0.2396765475166017</v>
+        <v>0.3253705590312893</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C110" t="n">
-        <v>0.3567813137069756</v>
+        <v>0.38108727062800274</v>
       </c>
       <c r="D110" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="B111" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C111" t="n">
-        <v>0.3866880282382423</v>
+        <v>0.2806994270505885</v>
       </c>
       <c r="D111" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="B112" t="s">
         <v>5</v>
       </c>
       <c r="C112" t="n">
-        <v>0.28654280100639445</v>
+        <v>0.108564306973777</v>
       </c>
       <c r="D112" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B113" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C113" t="n">
-        <v>0.39670845632675855</v>
+        <v>0.027871083217318182</v>
       </c>
       <c r="D113" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C114" t="n">
-        <v>0.21300619719447522</v>
+        <v>0.1482178289084472</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="B115" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C115" t="n">
-        <v>0.2614269101804163</v>
+        <v>0.36760106756412353</v>
       </c>
       <c r="D115" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116">
@@ -2218,13 +2206,13 @@
         <v>121</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C116" t="n">
-        <v>0.23733999875116696</v>
+        <v>0.38235958636283246</v>
       </c>
       <c r="D116" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117">
@@ -2232,27 +2220,27 @@
         <v>122</v>
       </c>
       <c r="B117" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C117" t="n">
-        <v>0.26794605521282056</v>
+        <v>0.3837582364904139</v>
       </c>
       <c r="D117" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B118" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1910689793142212</v>
+        <v>0.3423453232763452</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119">
@@ -2260,13 +2248,13 @@
         <v>123</v>
       </c>
       <c r="B119" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C119" t="n">
-        <v>0.16663775119290303</v>
+        <v>0.1187445089662345</v>
       </c>
       <c r="D119" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120">
@@ -2274,234 +2262,234 @@
         <v>124</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C120" t="n">
-        <v>0.3977897187210557</v>
+        <v>0.3484502582847829</v>
       </c>
       <c r="D120" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C121" t="n">
-        <v>0.32955754409243626</v>
+        <v>0.390289657973488</v>
       </c>
       <c r="D121" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B122" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C122" t="n">
-        <v>0.36917275513505987</v>
+        <v>0.3470059412680703</v>
       </c>
       <c r="D122" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C123" t="n">
-        <v>0.3226176792841277</v>
+        <v>0.25768560930183043</v>
       </c>
       <c r="D123" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="B124" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C124" t="n">
-        <v>0.14584723326725402</v>
+        <v>0.11374854282001434</v>
       </c>
       <c r="D124" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
       </c>
       <c r="C125" t="n">
-        <v>0.07031284896832517</v>
+        <v>0.3981047324961964</v>
       </c>
       <c r="D125" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B126" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C126" t="n">
-        <v>0.23532123296575252</v>
+        <v>0.22769162070882282</v>
       </c>
       <c r="D126" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>36</v>
       </c>
       <c r="B127" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C127" t="n">
-        <v>0.39398255562023543</v>
+        <v>0.2142189790153534</v>
       </c>
       <c r="D127" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C128" t="n">
-        <v>0.38257314479695936</v>
+        <v>0.3570974541261695</v>
       </c>
       <c r="D128" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C129" t="n">
-        <v>0.3844333552503279</v>
+        <v>0.3457319027252878</v>
       </c>
       <c r="D129" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
       </c>
       <c r="C130" t="n">
-        <v>0.3917511507815044</v>
+        <v>0.23188138640147207</v>
       </c>
       <c r="D130" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C131" t="n">
-        <v>0.38673983519022576</v>
+        <v>0.39278751721056177</v>
       </c>
       <c r="D131" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C132" t="n">
-        <v>0.3533272380877638</v>
+        <v>0.1455111829035462</v>
       </c>
       <c r="D132" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C133" t="n">
-        <v>0.28319841407871066</v>
+        <v>0.3929813928650322</v>
       </c>
       <c r="D133" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
       </c>
       <c r="C134" t="n">
-        <v>0.3904451811125395</v>
+        <v>0.23090430459012123</v>
       </c>
       <c r="D134" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C135" t="n">
-        <v>0.24039036861992308</v>
+        <v>0.39398740776299956</v>
       </c>
       <c r="D135" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C136" t="n">
-        <v>0.06990531703446949</v>
+        <v>0.3024945657620344</v>
       </c>
       <c r="D136" t="s">
         <v>24</v>
@@ -2509,44 +2497,44 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="B137" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C137" t="n">
-        <v>0.2763227643861643</v>
+        <v>0.36677987510853155</v>
       </c>
       <c r="D137" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C138" t="n">
-        <v>0.30362696690654895</v>
+        <v>0.3485315760211907</v>
       </c>
       <c r="D138" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C139" t="n">
-        <v>0.3930593593878309</v>
+        <v>0.35109814734970607</v>
       </c>
       <c r="D139" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140">
@@ -2554,150 +2542,150 @@
         <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C140" t="n">
-        <v>0.30439034353757916</v>
+        <v>0.1840503744692187</v>
       </c>
       <c r="D140" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C141" t="n">
-        <v>0.20658200086611256</v>
+        <v>0.048367741734063045</v>
       </c>
       <c r="D141" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C142" t="n">
-        <v>0.36453057416794016</v>
+        <v>0.3917997703652274</v>
       </c>
       <c r="D142" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C143" t="n">
-        <v>0.3004365296648358</v>
+        <v>0.04540213517876337</v>
       </c>
       <c r="D143" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C144" t="n">
-        <v>0.3907998448554058</v>
+        <v>0.37696088836088176</v>
       </c>
       <c r="D144" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C145" t="n">
-        <v>0.3535998956771629</v>
+        <v>0.3611795885493117</v>
       </c>
       <c r="D145" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C146" t="n">
-        <v>0.35606580963416</v>
+        <v>0.1337866014742023</v>
       </c>
       <c r="D146" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
       <c r="B147" t="s">
         <v>5</v>
       </c>
       <c r="C147" t="n">
-        <v>0.3959669563163377</v>
+        <v>0.3203917348152778</v>
       </c>
       <c r="D147" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C148" t="n">
-        <v>0.07040546995334297</v>
+        <v>0.25034373018886763</v>
       </c>
       <c r="D148" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C149" t="n">
-        <v>0.2538579119957754</v>
+        <v>0.28781589526339313</v>
       </c>
       <c r="D149" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C150" t="n">
-        <v>0.38205800796666495</v>
+        <v>0.3928487164262549</v>
       </c>
       <c r="D150" t="s">
         <v>20</v>
@@ -2705,13 +2693,13 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C151" t="n">
-        <v>0.2652339048707934</v>
+        <v>0.359334822151169</v>
       </c>
       <c r="D151" t="s">
         <v>22</v>
@@ -2719,41 +2707,41 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C152" t="n">
-        <v>0.23548695407179826</v>
+        <v>0.38305107487702605</v>
       </c>
       <c r="D152" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="B153" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C153" t="n">
-        <v>0.04747090857949223</v>
+        <v>0.30067560370898144</v>
       </c>
       <c r="D153" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B154" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C154" t="n">
-        <v>0.0061893469187460975</v>
+        <v>0.2402827142099178</v>
       </c>
       <c r="D154" t="s">
         <v>24</v>
@@ -2761,380 +2749,380 @@
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>155</v>
+        <v>83</v>
       </c>
       <c r="B155" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C155" t="n">
-        <v>0.04762344944969105</v>
+        <v>0.35907520556829725</v>
       </c>
       <c r="D155" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="B156" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C156" t="n">
-        <v>0.36575768702817174</v>
+        <v>0.13868713681582848</v>
       </c>
       <c r="D156" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C157" t="n">
-        <v>0.19632938983684106</v>
+        <v>0.38170717411526084</v>
       </c>
       <c r="D157" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B158" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C158" t="n">
-        <v>0.39517500123013066</v>
+        <v>0.12178851855999381</v>
       </c>
       <c r="D158" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B159" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C159" t="n">
-        <v>0.06659191292264513</v>
+        <v>0.39048833574447833</v>
       </c>
       <c r="D159" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C160" t="n">
-        <v>0.36461668166708905</v>
+        <v>0.0765309501823811</v>
       </c>
       <c r="D160" t="s">
-        <v>160</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
       </c>
       <c r="C161" t="n">
-        <v>0.3303638931236077</v>
+        <v>0.37615357518452974</v>
       </c>
       <c r="D161" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="B162" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C162" t="n">
-        <v>0.06803464524527708</v>
+        <v>0.1410652520613998</v>
       </c>
       <c r="D162" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="B163" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1408205624555954</v>
+        <v>0.1024251835908396</v>
       </c>
       <c r="D163" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="B164" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C164" t="n">
-        <v>0.3136449069450807</v>
+        <v>0.38468272501345163</v>
       </c>
       <c r="D164" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C165" t="n">
-        <v>0.13108752079002897</v>
+        <v>0.15841345977590288</v>
       </c>
       <c r="D165" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C166" t="n">
-        <v>0.3263681969645085</v>
+        <v>0.3957061533717947</v>
       </c>
       <c r="D166" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="B167" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C167" t="n">
-        <v>0.36703305017594656</v>
+        <v>0.3408823498110449</v>
       </c>
       <c r="D167" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B168" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C168" t="n">
-        <v>0.23135196801477606</v>
+        <v>0.1419411656589489</v>
       </c>
       <c r="D168" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B169" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C169" t="n">
-        <v>0.3956119359057037</v>
+        <v>0.33732960786966026</v>
       </c>
       <c r="D169" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
       </c>
       <c r="C170" t="n">
-        <v>0.29180652532217066</v>
+        <v>0.08913940893535027</v>
       </c>
       <c r="D170" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C171" t="n">
-        <v>0.38402836051169253</v>
+        <v>0.35266867189117745</v>
       </c>
       <c r="D171" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="B172" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C172" t="n">
-        <v>0.33653932310422474</v>
+        <v>0.13079041473158398</v>
       </c>
       <c r="D172" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C173" t="n">
-        <v>0.39894101528946674</v>
+        <v>0.15833022759860066</v>
       </c>
       <c r="D173" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B174" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C174" t="n">
-        <v>0.38024757201482773</v>
+        <v>0.34109581055458865</v>
       </c>
       <c r="D174" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C175" t="n">
-        <v>0.21656836994992607</v>
+        <v>0.3938848377602154</v>
       </c>
       <c r="D175" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C176" t="n">
-        <v>0.3950768180657239</v>
+        <v>0.024375451233784803</v>
       </c>
       <c r="D176" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="B177" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C177" t="n">
-        <v>0.10923742728828384</v>
+        <v>0.2748343890926546</v>
       </c>
       <c r="D177" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B178" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C178" t="n">
-        <v>0.29192765318103664</v>
+        <v>0.37749041399118927</v>
       </c>
       <c r="D178" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B179" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C179" t="n">
-        <v>0.26425384289109116</v>
+        <v>0.38217542186347697</v>
       </c>
       <c r="D179" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B180" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C180" t="n">
-        <v>0.3973872571280447</v>
+        <v>0.221166757240653</v>
       </c>
       <c r="D180" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>175</v>
+        <v>55</v>
       </c>
       <c r="B181" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C181" t="n">
-        <v>0.398026678525497</v>
+        <v>0.2659021714911606</v>
       </c>
       <c r="D181" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added CSVFileReader.java with methods to read Students and Projects, no bugs that i know of yet
</commit_message>
<xml_diff>
--- a/Analysis120.xlsx
+++ b/Analysis120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="175">
   <si>
     <t>Research Activity</t>
   </si>
@@ -26,508 +26,517 @@
     <t>Percentage Distribution</t>
   </si>
   <si>
-    <t>playing rock music</t>
+    <t>suing large corporations</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>0.92%</t>
+  </si>
+  <si>
+    <t>starring in romantic comedies</t>
+  </si>
+  <si>
+    <t>0.67%</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
+    <t>0.50%</t>
+  </si>
+  <si>
+    <t>writing beat fiction</t>
+  </si>
+  <si>
+    <t>creating monsters</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>solving mysteries</t>
+  </si>
+  <si>
+    <t>0.25%</t>
+  </si>
+  <si>
+    <t>singing blues songs</t>
+  </si>
+  <si>
+    <t>0.75%</t>
+  </si>
+  <si>
+    <t>writing TV comedies</t>
+  </si>
+  <si>
+    <t>0.08%</t>
+  </si>
+  <si>
+    <t>preaching to presidents</t>
+  </si>
+  <si>
+    <t>0.83%</t>
+  </si>
+  <si>
+    <t>interviewing politicians</t>
+  </si>
+  <si>
+    <t>0.42%</t>
+  </si>
+  <si>
+    <t>running a school for gifted teens</t>
+  </si>
+  <si>
+    <t>playing aggressive chess</t>
+  </si>
+  <si>
+    <t>0.33%</t>
+  </si>
+  <si>
+    <t>starring in pornographic movies</t>
+  </si>
+  <si>
     <t>0.17%</t>
   </si>
   <si>
+    <t>spreading revolution</t>
+  </si>
+  <si>
+    <t>campaigning for social causes</t>
+  </si>
+  <si>
+    <t>starring in madcap comedies</t>
+  </si>
+  <si>
+    <t>studying gorillas up close</t>
+  </si>
+  <si>
+    <t>telling epic tales</t>
+  </si>
+  <si>
+    <t>assassinating presidents</t>
+  </si>
+  <si>
+    <t>singing rock songs</t>
+  </si>
+  <si>
+    <t>0.58%</t>
+  </si>
+  <si>
+    <t>promoting Catholic values</t>
+  </si>
+  <si>
+    <t>posing for photographs</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>flaunting foppish fashions</t>
+  </si>
+  <si>
+    <t>making billions</t>
+  </si>
+  <si>
+    <t>playing the saxophone</t>
+  </si>
+  <si>
+    <t>starring in TV shows</t>
+  </si>
+  <si>
+    <t>pioneering new technologies</t>
+  </si>
+  <si>
+    <t>teaching the next generation</t>
+  </si>
+  <si>
+    <t>making unauthorized sex tapes</t>
+  </si>
+  <si>
+    <t>singing opera arias</t>
+  </si>
+  <si>
+    <t>1.00%</t>
+  </si>
+  <si>
+    <t>writing modern poetry</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes</t>
+  </si>
+  <si>
+    <t>telling dry jokes</t>
+  </si>
+  <si>
+    <t>winning battles</t>
+  </si>
+  <si>
+    <t>defending plaintiffs</t>
+  </si>
+  <si>
+    <t>running a tech giant</t>
+  </si>
+  <si>
+    <t>trading in wives</t>
+  </si>
+  <si>
+    <t>inventing electrical marvels</t>
+  </si>
+  <si>
+    <t>running an empire</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
+  </si>
+  <si>
+    <t>keeping a diary</t>
+  </si>
+  <si>
+    <t>singing melancholy songs</t>
+  </si>
+  <si>
+    <t>brokering peace deals</t>
+  </si>
+  <si>
+    <t>warning about totalitarianism</t>
+  </si>
+  <si>
+    <t>promoting greed</t>
+  </si>
+  <si>
+    <t>fighting civil wars</t>
+  </si>
+  <si>
+    <t>grabbing power</t>
+  </si>
+  <si>
+    <t>hiding from the public</t>
+  </si>
+  <si>
+    <t>clipping coupons</t>
+  </si>
+  <si>
+    <t>enriching uranium</t>
+  </si>
+  <si>
+    <t>dripping paint onto canvas</t>
+  </si>
+  <si>
+    <t>selling comic books</t>
+  </si>
+  <si>
+    <t>fighting the resistance</t>
+  </si>
+  <si>
+    <t>1.17%</t>
+  </si>
+  <si>
+    <t>suppressing violent urges</t>
+  </si>
+  <si>
+    <t>playing rock guitar</t>
+  </si>
+  <si>
+    <t>losing control</t>
+  </si>
+  <si>
+    <t>1.25%</t>
+  </si>
+  <si>
+    <t>fighting for civil rights</t>
+  </si>
+  <si>
+    <t>picking pockets</t>
+  </si>
+  <si>
+    <t>winning Michelin stars</t>
+  </si>
+  <si>
+    <t>making dunk shots</t>
+  </si>
+  <si>
+    <t>selling perfumes</t>
+  </si>
+  <si>
+    <t>planting daffodils</t>
+  </si>
+  <si>
+    <t>1.33%</t>
+  </si>
+  <si>
     <t>starring in Hollywood movies</t>
   </si>
   <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t>0.25%</t>
+    <t>singing Hipbop songs</t>
+  </si>
+  <si>
+    <t>gossiping with galpals</t>
+  </si>
+  <si>
+    <t>1.08%</t>
+  </si>
+  <si>
+    <t>making vulgar jokes</t>
+  </si>
+  <si>
+    <t>starring in comedies</t>
+  </si>
+  <si>
+    <t>competing in the Olympics</t>
+  </si>
+  <si>
+    <t>doing stand-up</t>
+  </si>
+  <si>
+    <t>promoting communism</t>
+  </si>
+  <si>
+    <t>writing experimental songs</t>
+  </si>
+  <si>
+    <t>causing mayhem</t>
+  </si>
+  <si>
+    <t>playing soccer</t>
+  </si>
+  <si>
+    <t>writing epic poetry</t>
+  </si>
+  <si>
+    <t>forging art</t>
+  </si>
+  <si>
+    <t>running a crime family</t>
+  </si>
+  <si>
+    <t>plotting strategies</t>
+  </si>
+  <si>
+    <t>ranting about politics</t>
+  </si>
+  <si>
+    <t>offering advice</t>
+  </si>
+  <si>
+    <t>manipulating political pawns</t>
+  </si>
+  <si>
+    <t>living amongst apes</t>
+  </si>
+  <si>
+    <t>turning it up to 11</t>
+  </si>
+  <si>
+    <t>playing God</t>
+  </si>
+  <si>
+    <t>climbing down chimneys</t>
+  </si>
+  <si>
+    <t>winning swimming competitions</t>
+  </si>
+  <si>
+    <t>arresting bootleggers</t>
+  </si>
+  <si>
+    <t>making strategic decisions</t>
+  </si>
+  <si>
+    <t>studying magic tricks</t>
+  </si>
+  <si>
+    <t>running film festivals</t>
+  </si>
+  <si>
+    <t>solving riddles</t>
+  </si>
+  <si>
+    <t>losing court cases</t>
+  </si>
+  <si>
+    <t>running theme parks</t>
+  </si>
+  <si>
+    <t>throwing fund-raisers for Parkinson's disease</t>
+  </si>
+  <si>
+    <t>commanding a spaceship</t>
+  </si>
+  <si>
+    <t>searching for the messiah</t>
+  </si>
+  <si>
+    <t>1.42%</t>
+  </si>
+  <si>
+    <t>exploring darkest Africa</t>
+  </si>
+  <si>
+    <t>collecting rock samples</t>
+  </si>
+  <si>
+    <t>avoiding growing old</t>
+  </si>
+  <si>
+    <t>singing parody songs</t>
+  </si>
+  <si>
+    <t>duelling acrobatically</t>
+  </si>
+  <si>
+    <t>writing plays about the middle classes</t>
+  </si>
+  <si>
+    <t>spying for the enemy</t>
+  </si>
+  <si>
+    <t>winning boxing matches</t>
+  </si>
+  <si>
+    <t>battling the forces of darkness</t>
+  </si>
+  <si>
+    <t>creating dictionaries</t>
+  </si>
+  <si>
+    <t>studying science</t>
+  </si>
+  <si>
+    <t>cleaning floors</t>
+  </si>
+  <si>
+    <t>climbing social ladders</t>
+  </si>
+  <si>
+    <t>seducing women</t>
+  </si>
+  <si>
+    <t>doing raunchy stage acts</t>
+  </si>
+  <si>
+    <t>looking after children</t>
+  </si>
+  <si>
+    <t>seducing young women</t>
+  </si>
+  <si>
+    <t>writing erotic fiction</t>
+  </si>
+  <si>
+    <t>walking like a man</t>
+  </si>
+  <si>
+    <t>finding clues</t>
+  </si>
+  <si>
+    <t>developing military strategies</t>
+  </si>
+  <si>
+    <t>abusing power</t>
+  </si>
+  <si>
+    <t>instigating rebellion</t>
+  </si>
+  <si>
+    <t>running a frontier town</t>
+  </si>
+  <si>
+    <t>campaigning for democracy</t>
+  </si>
+  <si>
+    <t>setting mousetraps</t>
+  </si>
+  <si>
+    <t>writing funny movies</t>
+  </si>
+  <si>
+    <t>directing the business of state</t>
+  </si>
+  <si>
+    <t>analyzing the sub-conscious</t>
+  </si>
+  <si>
+    <t>spreading political gossip</t>
+  </si>
+  <si>
+    <t>fussing about cleanliness</t>
+  </si>
+  <si>
+    <t>pursuing criminals</t>
+  </si>
+  <si>
+    <t>directing animated films</t>
+  </si>
+  <si>
+    <t>promoting pop music</t>
+  </si>
+  <si>
+    <t>preparing for the apocalypse</t>
+  </si>
+  <si>
+    <t>telling tall tales</t>
+  </si>
+  <si>
+    <t>manipulating ingenues</t>
+  </si>
+  <si>
+    <t>cheating at poker</t>
+  </si>
+  <si>
+    <t>selling airline seats</t>
+  </si>
+  <si>
+    <t>peacocking in fancy clothes</t>
+  </si>
+  <si>
+    <t>playing James Bond</t>
+  </si>
+  <si>
+    <t>running a business empire</t>
+  </si>
+  <si>
+    <t>fighting with the mob</t>
+  </si>
+  <si>
+    <t>guarding the galaxy</t>
+  </si>
+  <si>
+    <t>fighting with swords</t>
+  </si>
+  <si>
+    <t>exorcising demons</t>
+  </si>
+  <si>
+    <t>issuing fatwas</t>
+  </si>
+  <si>
+    <t>promoting racial harmony</t>
+  </si>
+  <si>
+    <t>preaching tolerance</t>
+  </si>
+  <si>
+    <t>playing the organ</t>
   </si>
   <si>
     <t>moaning about men</t>
   </si>
   <si>
-    <t>0.42%</t>
-  </si>
-  <si>
-    <t>making action movies</t>
-  </si>
-  <si>
-    <t>writing comedy</t>
-  </si>
-  <si>
-    <t>0.92%</t>
-  </si>
-  <si>
-    <t>running a multinational corporation</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>1.42%</t>
-  </si>
-  <si>
-    <t>singing torch songs</t>
-  </si>
-  <si>
-    <t>promoting greed</t>
-  </si>
-  <si>
-    <t>0.67%</t>
-  </si>
-  <si>
-    <t>handing out flowers</t>
-  </si>
-  <si>
-    <t>1.00%</t>
-  </si>
-  <si>
-    <t>playing basketball</t>
-  </si>
-  <si>
-    <t>0.58%</t>
-  </si>
-  <si>
-    <t>ranting about liberals</t>
-  </si>
-  <si>
-    <t>painting colorful pictures</t>
-  </si>
-  <si>
-    <t>0.50%</t>
-  </si>
-  <si>
-    <t>writing plays</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes</t>
-  </si>
-  <si>
-    <t>promoting liberal values</t>
-  </si>
-  <si>
-    <t>commenting on social issues</t>
-  </si>
-  <si>
-    <t>preparing for war</t>
-  </si>
-  <si>
-    <t>fighting the resistance</t>
-  </si>
-  <si>
-    <t>reporting for The Daily Planet</t>
-  </si>
-  <si>
-    <t>0.83%</t>
-  </si>
-  <si>
-    <t>promoting conservative values</t>
-  </si>
-  <si>
-    <t>0.33%</t>
-  </si>
-  <si>
-    <t>0.08%</t>
-  </si>
-  <si>
-    <t>punching out Nazis</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
-    <t>studying magic tricks</t>
-  </si>
-  <si>
-    <t>seducing emperors</t>
-  </si>
-  <si>
-    <t>throwing sex parties</t>
-  </si>
-  <si>
-    <t>selling consumer goods</t>
-  </si>
-  <si>
-    <t>seeking revenge</t>
-  </si>
-  <si>
-    <t>inventing electrical marvels</t>
-  </si>
-  <si>
-    <t>lecturing about climate change</t>
-  </si>
-  <si>
-    <t>pioneering new technologies</t>
-  </si>
-  <si>
-    <t>writing about sex</t>
-  </si>
-  <si>
-    <t>watching the sun rise</t>
-  </si>
-  <si>
-    <t>0.75%</t>
-  </si>
-  <si>
-    <t>writing TV comedies</t>
-  </si>
-  <si>
-    <t>promoting Eastern philosophy</t>
-  </si>
-  <si>
-    <t>composing classical music</t>
-  </si>
-  <si>
-    <t>promoting hair products</t>
-  </si>
-  <si>
-    <t>fighting for the rebel alliance</t>
-  </si>
-  <si>
-    <t>singing pop songs</t>
-  </si>
-  <si>
-    <t>testing scientific theories</t>
-  </si>
-  <si>
-    <t>chasing starlets</t>
-  </si>
-  <si>
-    <t>defending plaintiffs</t>
-  </si>
-  <si>
-    <t>playing soccer</t>
-  </si>
-  <si>
-    <t>designing clothes</t>
-  </si>
-  <si>
-    <t>carrying secret plans</t>
-  </si>
-  <si>
-    <t>starring in action movies</t>
-  </si>
-  <si>
-    <t>working for the forces of darkness</t>
-  </si>
-  <si>
-    <t>insulting minorities</t>
-  </si>
-  <si>
-    <t>killing people in ingenious ways</t>
-  </si>
-  <si>
-    <t>chasing criminals</t>
-  </si>
-  <si>
-    <t>1.08%</t>
+    <t>falling in love</t>
+  </si>
+  <si>
+    <t>avenging loved ones</t>
   </si>
   <si>
     <t>counting tooth picks</t>
   </si>
   <si>
-    <t>solving mysteries</t>
-  </si>
-  <si>
-    <t>1.33%</t>
-  </si>
-  <si>
-    <t>fighting for civil rights</t>
-  </si>
-  <si>
-    <t>singing to teenagers</t>
-  </si>
-  <si>
-    <t>piloting the Millenium Falcon</t>
-  </si>
-  <si>
-    <t>offering advice</t>
-  </si>
-  <si>
-    <t>finding clues</t>
-  </si>
-  <si>
-    <t>leading revolts</t>
-  </si>
-  <si>
-    <t>1.25%</t>
-  </si>
-  <si>
-    <t>writing modern fiction</t>
-  </si>
-  <si>
-    <t>developing new technologies</t>
-  </si>
-  <si>
-    <t>flying into a rage</t>
-  </si>
-  <si>
-    <t>writing pop songs</t>
-  </si>
-  <si>
-    <t>running a business empire</t>
-  </si>
-  <si>
-    <t>making dumb comedies</t>
-  </si>
-  <si>
-    <t>writing about manly pursuits</t>
-  </si>
-  <si>
-    <t>running an empire</t>
-  </si>
-  <si>
-    <t>bodybuilding</t>
-  </si>
-  <si>
-    <t>representing criminals</t>
-  </si>
-  <si>
-    <t>smuggling contraband</t>
-  </si>
-  <si>
-    <t>1.17%</t>
-  </si>
-  <si>
-    <t>singing experimental songs</t>
-  </si>
-  <si>
     <t>exploring foreign countries</t>
-  </si>
-  <si>
-    <t>doing stand-up</t>
-  </si>
-  <si>
-    <t>robbing banks</t>
-  </si>
-  <si>
-    <t>starring in reality TV shows</t>
-  </si>
-  <si>
-    <t>campaigning for world peace</t>
-  </si>
-  <si>
-    <t>recording pop songs</t>
-  </si>
-  <si>
-    <t>writing short stories</t>
-  </si>
-  <si>
-    <t>promoting communism</t>
-  </si>
-  <si>
-    <t>recruiting dissidents</t>
-  </si>
-  <si>
-    <t>peacocking in fancy clothes</t>
-  </si>
-  <si>
-    <t>opening new markets</t>
-  </si>
-  <si>
-    <t>driving under the influence</t>
-  </si>
-  <si>
-    <t>building houses for poor people</t>
-  </si>
-  <si>
-    <t>making trains run on time</t>
-  </si>
-  <si>
-    <t>developing operating systems</t>
-  </si>
-  <si>
-    <t>performing physical therapy</t>
-  </si>
-  <si>
-    <t>pulling dirty political tricks</t>
-  </si>
-  <si>
-    <t>pedalling furiously</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>frying crabby patties</t>
-  </si>
-  <si>
-    <t>promoting Fascism</t>
-  </si>
-  <si>
-    <t>looking for love</t>
-  </si>
-  <si>
-    <t>developing advertising campaigns</t>
-  </si>
-  <si>
-    <t>writing plays about the middle classes</t>
-  </si>
-  <si>
-    <t>eluding electronic ghosts</t>
-  </si>
-  <si>
-    <t>spouting movie trivia</t>
-  </si>
-  <si>
-    <t>studying science</t>
-  </si>
-  <si>
-    <t>preaching to presidents</t>
-  </si>
-  <si>
-    <t>promoting logical thinking</t>
-  </si>
-  <si>
-    <t>plotting election strategies</t>
-  </si>
-  <si>
-    <t>convicting criminals</t>
-  </si>
-  <si>
-    <t>promoting air travel</t>
-  </si>
-  <si>
-    <t>complaining about everything</t>
-  </si>
-  <si>
-    <t>assassinating presidents</t>
-  </si>
-  <si>
-    <t>preventing terrorism</t>
-  </si>
-  <si>
-    <t>podcasting about movies</t>
-  </si>
-  <si>
-    <t>running a technology company</t>
-  </si>
-  <si>
-    <t>writing in ledgers</t>
-  </si>
-  <si>
-    <t>suppressing violent urges</t>
-  </si>
-  <si>
-    <t>running a media empire</t>
-  </si>
-  <si>
-    <t>promoting capitalism</t>
-  </si>
-  <si>
-    <t>foiling the schemes of evil villains</t>
-  </si>
-  <si>
-    <t>wielding political power</t>
-  </si>
-  <si>
-    <t>teaching philosophy</t>
-  </si>
-  <si>
-    <t>painting realistic pictures</t>
-  </si>
-  <si>
-    <t>escaping from water tanks</t>
-  </si>
-  <si>
-    <t>avoiding paparazzi</t>
-  </si>
-  <si>
-    <t>preventing crime</t>
-  </si>
-  <si>
-    <t>chasing flappers</t>
-  </si>
-  <si>
-    <t>drawing whimsical cartoons</t>
-  </si>
-  <si>
-    <t>playing tough guys</t>
-  </si>
-  <si>
-    <t>writing mystery stories</t>
-  </si>
-  <si>
-    <t>smoking herb</t>
-  </si>
-  <si>
-    <t>moaning about women</t>
-  </si>
-  <si>
-    <t>killing murderers</t>
-  </si>
-  <si>
-    <t>singing country music</t>
-  </si>
-  <si>
-    <t>running a large metropolitan city</t>
-  </si>
-  <si>
-    <t>climbing social ladders</t>
-  </si>
-  <si>
-    <t>developing military strategies</t>
-  </si>
-  <si>
-    <t>fighting with swords</t>
-  </si>
-  <si>
-    <t>singing melancholy songs</t>
-  </si>
-  <si>
-    <t>running a criminal empire</t>
-  </si>
-  <si>
-    <t>building rocket ships</t>
-  </si>
-  <si>
-    <t>winning Michelin stars</t>
-  </si>
-  <si>
-    <t>writing poetry</t>
-  </si>
-  <si>
-    <t>instigating rebellion</t>
-  </si>
-  <si>
-    <t>inventing new technologies</t>
-  </si>
-  <si>
-    <t>racking up marriages</t>
-  </si>
-  <si>
-    <t>painting dark pictures</t>
-  </si>
-  <si>
-    <t>following the money</t>
-  </si>
-  <si>
-    <t>falling gracefully</t>
-  </si>
-  <si>
-    <t>offering medical opinions</t>
-  </si>
-  <si>
-    <t>leaking classified documents</t>
-  </si>
-  <si>
-    <t>making fantasy movies</t>
-  </si>
-  <si>
-    <t>investigating alien abductions</t>
-  </si>
-  <si>
-    <t>making escape plans</t>
-  </si>
-  <si>
-    <t>being a good neighbor</t>
-  </si>
-  <si>
-    <t>duelling acrobatically</t>
-  </si>
-  <si>
-    <t>building a search engine</t>
   </si>
 </sst>
 </file>
@@ -585,10 +594,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="34.9609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="9.69921875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.85546875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="28.9375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="37.46875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.11328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="27.51953125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -613,7 +622,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.12365953745407593</v>
+        <v>0.3771525118200255</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -624,24 +633,24 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3646255019797833</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.3081660877607913</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0.36716977630315917</v>
+        <v>0.255604520663135</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -652,13 +661,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.17221262028805595</v>
+        <v>0.39855096910266485</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -666,13 +675,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2655117594509621</v>
+        <v>0.388105506826859</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -680,27 +689,27 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.09675692324692625</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.38845540188193356</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.37411378586688787</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.03288585961340481</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -708,10 +717,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>0.24978323433855135</v>
+        <v>0.12758496465270888</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -722,10 +731,10 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3086112101385406</v>
+        <v>0.3926282967706807</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -736,10 +745,10 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3461643239938675</v>
+        <v>0.1500881269848936</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -750,13 +759,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>0.39132421848624854</v>
+        <v>0.22290217075841404</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -764,10 +773,10 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" t="n">
-        <v>0.25481152457306144</v>
+        <v>0.38501546614117244</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -778,192 +787,192 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>0.30897974719167964</v>
+        <v>0.09671525303963519</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>0.38259560949729304</v>
+        <v>0.39350458851137604</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3901038070756383</v>
+        <v>0.2815999764677612</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>0.35457822594702904</v>
+        <v>0.39850952592190614</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>0.27788817386895714</v>
+        <v>0.1700007606877913</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.09147267907267095</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.35352196312379774</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.27811472405602516</v>
+        <v>0.14788062035783547</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.38112907723153805</v>
+      </c>
+      <c r="D21" t="s">
         <v>8</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.2887532183039643</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C22" t="n">
-        <v>0.12766579764148503</v>
+        <v>0.3750041096359953</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.39015153967339955</v>
+        <v>0.29165648462817423</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3892826310584495</v>
+        <v>0.007791466886580667</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01516138471618333</v>
+        <v>0.21703594955967992</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
-        <v>0.38994686380694266</v>
+        <v>0.3149894115271835</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>0.10526104554650073</v>
+        <v>0.36087195461953875</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -971,13 +980,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>0.26093907813436523</v>
+        <v>0.39852341427127824</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -988,13 +997,13 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>0.18584677865155758</v>
+        <v>0.3988341899937757</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30">
@@ -1002,13 +1011,13 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3981158216832802</v>
+        <v>0.3579884829480844</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -1016,13 +1025,13 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2949012128340598</v>
+        <v>0.27621421844493715</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1030,13 +1039,13 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32" t="n">
-        <v>0.25259837387002093</v>
+        <v>0.39257258315500143</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
@@ -1044,13 +1053,13 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>0.37677821407813844</v>
+        <v>0.3903961138515097</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34">
@@ -1058,55 +1067,55 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>0.23324768784803546</v>
+        <v>0.37158550587196204</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C35" t="n">
-        <v>0.3067249494379602</v>
+        <v>0.39609459835435085</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.26105776079742954</v>
+      </c>
+      <c r="D36" t="s">
         <v>16</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.3400192858795854</v>
-      </c>
-      <c r="D36" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1969789147883943</v>
+        <v>0.052344178983057384</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38">
@@ -1114,13 +1123,13 @@
         <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C38" t="n">
-        <v>0.2364629732325973</v>
+        <v>0.16007345584935626</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39">
@@ -1128,10 +1137,10 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1963999777565019</v>
+        <v>0.23491068183550962</v>
       </c>
       <c r="D39" t="s">
         <v>27</v>
@@ -1142,13 +1151,13 @@
         <v>54</v>
       </c>
       <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.3438042307426023</v>
+      </c>
+      <c r="D40" t="s">
         <v>8</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0.11671925738023523</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="41">
@@ -1156,13 +1165,13 @@
         <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C41" t="n">
-        <v>0.36071431386035857</v>
+        <v>0.11635006788537892</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42">
@@ -1170,13 +1179,13 @@
         <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C42" t="n">
-        <v>0.3224424896438208</v>
+        <v>0.35460801021166716</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43">
@@ -1184,13 +1193,13 @@
         <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C43" t="n">
-        <v>0.19933285509828066</v>
+        <v>0.12951637466057678</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
@@ -1198,13 +1207,13 @@
         <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C44" t="n">
-        <v>0.08083283693597261</v>
+        <v>0.30702363753132356</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45">
@@ -1212,13 +1221,13 @@
         <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C45" t="n">
-        <v>0.34903379663558254</v>
+        <v>0.2948680118341556</v>
       </c>
       <c r="D45" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46">
@@ -1226,10 +1235,10 @@
         <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C46" t="n">
-        <v>0.3989139469669982</v>
+        <v>0.16421422967457672</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
@@ -1243,10 +1252,10 @@
         <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.18810862037542894</v>
+        <v>0.360713655672053</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48">
@@ -1254,13 +1263,13 @@
         <v>62</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.347740007437327</v>
+        <v>0.10313488311457508</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49">
@@ -1268,13 +1277,13 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>0.3921122762843404</v>
+        <v>0.2504716916054045</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -1282,83 +1291,83 @@
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C50" t="n">
-        <v>0.24421794261879945</v>
+        <v>0.11760559881202408</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>0.36509615466475986</v>
+        <v>0.008079313274094096</v>
       </c>
       <c r="D51" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C52" t="n">
-        <v>0.13912601209466585</v>
+        <v>0.3943773182159054</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>0.152706692845559</v>
+        <v>0.23321148571638758</v>
       </c>
       <c r="D53" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.15169143052674494</v>
+      </c>
+      <c r="D54" t="s">
         <v>16</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0.3939916535312771</v>
-      </c>
-      <c r="D54" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C55" t="n">
-        <v>0.2748630531424906</v>
+        <v>0.1522172195863736</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
@@ -1366,209 +1375,209 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C56" t="n">
-        <v>0.39876792017613866</v>
+        <v>0.3260413761879838</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C57" t="n">
-        <v>0.3663865152402292</v>
+        <v>0.2927306117747792</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C58" t="n">
-        <v>0.3986635675595113</v>
+        <v>0.3707107397019012</v>
       </c>
       <c r="D58" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C59" t="n">
-        <v>0.20571368375477841</v>
+        <v>0.03780251639704063</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C60" t="n">
-        <v>0.3548975411742942</v>
+        <v>0.04258837114393448</v>
       </c>
       <c r="D60" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C61" t="n">
-        <v>0.07476486079881246</v>
+        <v>0.3910241760657666</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C62" t="n">
-        <v>0.3520112472582488</v>
+        <v>0.11930650046219593</v>
       </c>
       <c r="D62" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3517973635248737</v>
+        <v>0.35064425483769696</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C64" t="n">
-        <v>0.07993519948598601</v>
+        <v>0.19220817712851088</v>
       </c>
       <c r="D64" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3962334563097132</v>
+        <v>0.3030941823190015</v>
       </c>
       <c r="D65" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>0.39316243326708006</v>
+        <v>0.2797147654195351</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C67" t="n">
-        <v>0.2485267459194358</v>
+        <v>0.12931253220924038</v>
       </c>
       <c r="D67" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C68" t="n">
-        <v>0.17937095351282456</v>
+        <v>0.20633838793970785</v>
       </c>
       <c r="D68" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69" t="n">
-        <v>0.003170425617031888</v>
+        <v>0.37704895531483745</v>
       </c>
       <c r="D69" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.3526339359971409</v>
+      </c>
+      <c r="D70" t="s">
         <v>84</v>
-      </c>
-      <c r="B70" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0.13268138930978596</v>
-      </c>
-      <c r="D70" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="71">
@@ -1576,13 +1585,13 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C71" t="n">
-        <v>0.3980529481707508</v>
+        <v>0.39014248126527284</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72">
@@ -1590,276 +1599,276 @@
         <v>86</v>
       </c>
       <c r="B72" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C72" t="n">
-        <v>0.3380708317513376</v>
+        <v>0.2230534173834142</v>
       </c>
       <c r="D72" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C73" t="n">
-        <v>0.27693515359107357</v>
+        <v>0.3545240444591294</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C74" t="n">
-        <v>0.07046566766835163</v>
+        <v>0.27018722764482594</v>
       </c>
       <c r="D74" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C75" t="n">
-        <v>0.39838279261407145</v>
+        <v>0.21586387809319296</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2660149345362879</v>
+        <v>0.3674665698368085</v>
       </c>
       <c r="D76" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>0.05861664668347628</v>
+        <v>0.3697159583114312</v>
       </c>
       <c r="D77" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C78" t="n">
-        <v>0.12755064387338266</v>
+        <v>0.16683323785450918</v>
       </c>
       <c r="D78" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C79" t="n">
-        <v>0.39883739011868574</v>
+        <v>0.2583412038093409</v>
       </c>
       <c r="D79" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C80" t="n">
-        <v>0.38120672526689475</v>
+        <v>0.387729515692608</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="C81" t="n">
-        <v>0.34338774094644026</v>
+        <v>0.39839934009451644</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
       </c>
       <c r="C82" t="n">
-        <v>0.21774113798309477</v>
+        <v>0.12637977946021792</v>
       </c>
       <c r="D82" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3519214270761913</v>
+        <v>0.16393244269134918</v>
       </c>
       <c r="D83" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B84" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C84" t="n">
-        <v>0.04863864293838953</v>
+        <v>0.37904591389936687</v>
       </c>
       <c r="D84" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C85" t="n">
-        <v>0.3890763265647619</v>
+        <v>0.3974562484797686</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
       <c r="C86" t="n">
-        <v>0.3786112961307445</v>
+        <v>0.11193857033695064</v>
       </c>
       <c r="D86" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
       <c r="C87" t="n">
-        <v>0.3123177750385231</v>
+        <v>0.39464737901511876</v>
       </c>
       <c r="D87" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C88" t="n">
-        <v>0.3529212435730347</v>
+        <v>0.21962218538002148</v>
       </c>
       <c r="D88" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C89" t="n">
-        <v>0.09227333916875784</v>
+        <v>0.3326842355438256</v>
       </c>
       <c r="D89" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C90" t="n">
-        <v>0.3985993715745561</v>
+        <v>0.1932607567866209</v>
       </c>
       <c r="D90" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>0.39747431251602994</v>
+        <v>0.24743536451615375</v>
       </c>
       <c r="D91" t="s">
         <v>24</v>
@@ -1867,100 +1876,100 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
       </c>
       <c r="C92" t="n">
-        <v>0.2648311974789042</v>
+        <v>0.36823729671489497</v>
       </c>
       <c r="D92" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C93" t="n">
-        <v>0.3579013315330324</v>
+        <v>0.07070116960420744</v>
       </c>
       <c r="D93" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C94" t="n">
-        <v>0.3034873180936606</v>
+        <v>0.3986312601205356</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C95" t="n">
-        <v>0.36699602062983994</v>
+        <v>0.1738155154936748</v>
       </c>
       <c r="D95" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C96" t="n">
-        <v>0.25897535143439976</v>
+        <v>0.3864857911832088</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C97" t="n">
-        <v>0.39890444248500023</v>
+        <v>0.3203700060056968</v>
       </c>
       <c r="D97" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C98" t="n">
-        <v>0.09011786084235188</v>
+        <v>0.21557862302049197</v>
       </c>
       <c r="D98" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="99">
@@ -1968,41 +1977,41 @@
         <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C99" t="n">
-        <v>0.38733628824757993</v>
+        <v>0.09365391903615662</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C100" t="n">
-        <v>0.36507778600493346</v>
+        <v>0.3912132765051571</v>
       </c>
       <c r="D100" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B101" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C101" t="n">
-        <v>0.29981050018305444</v>
+        <v>0.3673221310241492</v>
       </c>
       <c r="D101" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102">
@@ -2010,10 +2019,10 @@
         <v>111</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C102" t="n">
-        <v>0.30427328177379676</v>
+        <v>0.3474446539937292</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
@@ -2024,10 +2033,10 @@
         <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C103" t="n">
-        <v>0.16128021956448022</v>
+        <v>0.12902478428653474</v>
       </c>
       <c r="D103" t="s">
         <v>20</v>
@@ -2038,587 +2047,587 @@
         <v>113</v>
       </c>
       <c r="B104" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C104" t="n">
-        <v>0.37084387925311324</v>
+        <v>0.3466071608131492</v>
       </c>
       <c r="D104" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C105" t="n">
-        <v>0.3640868339126881</v>
+        <v>0.3966350569353832</v>
       </c>
       <c r="D105" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C106" t="n">
-        <v>0.26916621081657593</v>
+        <v>0.31534200744168117</v>
       </c>
       <c r="D106" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B107" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.2927572815908294</v>
+      </c>
+      <c r="D107" t="s">
         <v>8</v>
-      </c>
-      <c r="C107" t="n">
-        <v>0.395038162282362</v>
-      </c>
-      <c r="D107" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B108" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C108" t="n">
-        <v>0.22324043306376562</v>
+        <v>0.16223763462710555</v>
       </c>
       <c r="D108" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="B109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0.1887011488739992</v>
+      </c>
+      <c r="D109" t="s">
         <v>16</v>
-      </c>
-      <c r="C109" t="n">
-        <v>0.3253705590312893</v>
-      </c>
-      <c r="D109" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C110" t="n">
-        <v>0.38108727062800274</v>
+        <v>0.26507535903354684</v>
       </c>
       <c r="D110" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C111" t="n">
-        <v>0.2806994270505885</v>
+        <v>0.152007053310442</v>
       </c>
       <c r="D111" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C112" t="n">
-        <v>0.108564306973777</v>
+        <v>0.34861892203892547</v>
       </c>
       <c r="D112" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B113" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C113" t="n">
-        <v>0.027871083217318182</v>
+        <v>0.3979525123671936</v>
       </c>
       <c r="D113" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1482178289084472</v>
+        <v>0.23263872870350708</v>
       </c>
       <c r="D114" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B115" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C115" t="n">
-        <v>0.36760106756412353</v>
+        <v>0.1284531072635669</v>
       </c>
       <c r="D115" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B116" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C116" t="n">
-        <v>0.38235958636283246</v>
+        <v>0.16251453160036733</v>
       </c>
       <c r="D116" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C117" t="n">
-        <v>0.3837582364904139</v>
+        <v>0.20316774526260142</v>
       </c>
       <c r="D117" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
       </c>
       <c r="C118" t="n">
-        <v>0.3423453232763452</v>
+        <v>0.3458699515754768</v>
       </c>
       <c r="D118" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B119" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1187445089662345</v>
+        <v>0.3946435663698323</v>
       </c>
       <c r="D119" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C120" t="n">
-        <v>0.3484502582847829</v>
+        <v>0.39828653159282507</v>
       </c>
       <c r="D120" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B121" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C121" t="n">
-        <v>0.390289657973488</v>
+        <v>0.11324385868196526</v>
       </c>
       <c r="D121" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B122" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C122" t="n">
-        <v>0.3470059412680703</v>
+        <v>0.3482862173983848</v>
       </c>
       <c r="D122" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
       <c r="B123" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C123" t="n">
-        <v>0.25768560930183043</v>
+        <v>0.06573755020454998</v>
       </c>
       <c r="D123" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B124" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C124" t="n">
-        <v>0.11374854282001434</v>
+        <v>0.32208320035144833</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C125" t="n">
-        <v>0.3981047324961964</v>
+        <v>0.30970764546054863</v>
       </c>
       <c r="D125" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C126" t="n">
-        <v>0.22769162070882282</v>
+        <v>0.37966208728211054</v>
       </c>
       <c r="D126" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
       </c>
       <c r="C127" t="n">
-        <v>0.2142189790153534</v>
+        <v>0.3979699876987751</v>
       </c>
       <c r="D127" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C128" t="n">
-        <v>0.3570974541261695</v>
+        <v>0.3340889962145578</v>
       </c>
       <c r="D128" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C129" t="n">
-        <v>0.3457319027252878</v>
+        <v>0.3453402887458102</v>
       </c>
       <c r="D129" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C130" t="n">
-        <v>0.23188138640147207</v>
+        <v>0.37023232824712726</v>
       </c>
       <c r="D130" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C131" t="n">
-        <v>0.39278751721056177</v>
+        <v>0.2736153602960227</v>
       </c>
       <c r="D131" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1455111829035462</v>
+        <v>0.3161669184150581</v>
       </c>
       <c r="D132" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B133" t="s">
+        <v>14</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0.24799123771051684</v>
+      </c>
+      <c r="D133" t="s">
         <v>16</v>
-      </c>
-      <c r="C133" t="n">
-        <v>0.3929813928650322</v>
-      </c>
-      <c r="D133" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C134" t="n">
-        <v>0.23090430459012123</v>
+        <v>0.38692295539842</v>
       </c>
       <c r="D134" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C135" t="n">
-        <v>0.39398740776299956</v>
+        <v>0.22800464062382342</v>
       </c>
       <c r="D135" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B136" t="s">
         <v>5</v>
       </c>
       <c r="C136" t="n">
-        <v>0.3024945657620344</v>
+        <v>0.39753694486923696</v>
       </c>
       <c r="D136" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C137" t="n">
-        <v>0.36677987510853155</v>
+        <v>0.2443168207760745</v>
       </c>
       <c r="D137" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B138" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0.3227197183652633</v>
+      </c>
+      <c r="D138" t="s">
         <v>8</v>
-      </c>
-      <c r="C138" t="n">
-        <v>0.3485315760211907</v>
-      </c>
-      <c r="D138" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C139" t="n">
-        <v>0.35109814734970607</v>
+        <v>0.38372251675728947</v>
       </c>
       <c r="D139" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.2857144451806134</v>
+      </c>
+      <c r="D140" t="s">
         <v>16</v>
-      </c>
-      <c r="C140" t="n">
-        <v>0.1840503744692187</v>
-      </c>
-      <c r="D140" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B141" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.3976438750684375</v>
+      </c>
+      <c r="D141" t="s">
         <v>16</v>
-      </c>
-      <c r="C141" t="n">
-        <v>0.048367741734063045</v>
-      </c>
-      <c r="D141" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C142" t="n">
-        <v>0.3917997703652274</v>
+        <v>0.3838826112883563</v>
       </c>
       <c r="D142" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C143" t="n">
-        <v>0.04540213517876337</v>
+        <v>0.3885958780319866</v>
       </c>
       <c r="D143" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C144" t="n">
-        <v>0.37696088836088176</v>
+        <v>0.23958594151700613</v>
       </c>
       <c r="D144" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>145</v>
+        <v>48</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C145" t="n">
-        <v>0.3611795885493117</v>
+        <v>0.2067229834447565</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146">
@@ -2626,503 +2635,503 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1337866014742023</v>
+        <v>0.39746341077488334</v>
       </c>
       <c r="D146" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C147" t="n">
-        <v>0.3203917348152778</v>
+        <v>0.37103420123441366</v>
       </c>
       <c r="D147" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C148" t="n">
-        <v>0.25034373018886763</v>
+        <v>0.3737802674008737</v>
       </c>
       <c r="D148" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C149" t="n">
-        <v>0.28781589526339313</v>
+        <v>0.3979182935798989</v>
       </c>
       <c r="D149" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C150" t="n">
-        <v>0.3928487164262549</v>
+        <v>0.3031618774352718</v>
       </c>
       <c r="D150" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C151" t="n">
-        <v>0.359334822151169</v>
+        <v>0.22634113260693386</v>
       </c>
       <c r="D151" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="B152" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C152" t="n">
-        <v>0.38305107487702605</v>
+        <v>0.3917762702589316</v>
       </c>
       <c r="D152" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="B153" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C153" t="n">
-        <v>0.30067560370898144</v>
+        <v>0.3866718949828442</v>
       </c>
       <c r="D153" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C154" t="n">
-        <v>0.2402827142099178</v>
+        <v>0.1906118732119003</v>
       </c>
       <c r="D154" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C155" t="n">
-        <v>0.35907520556829725</v>
+        <v>0.38755547477371777</v>
       </c>
       <c r="D155" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>71</v>
+        <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C156" t="n">
-        <v>0.13868713681582848</v>
+        <v>0.06172094937285739</v>
       </c>
       <c r="D156" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C157" t="n">
-        <v>0.38170717411526084</v>
+        <v>0.052606664584758996</v>
       </c>
       <c r="D157" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B158" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0.23579486220019882</v>
+      </c>
+      <c r="D158" t="s">
         <v>8</v>
-      </c>
-      <c r="C158" t="n">
-        <v>0.12178851855999381</v>
-      </c>
-      <c r="D158" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C159" t="n">
-        <v>0.39048833574447833</v>
+        <v>0.39077914514837986</v>
       </c>
       <c r="D159" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="B160" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C160" t="n">
-        <v>0.0765309501823811</v>
+        <v>0.3695226962670783</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
       </c>
       <c r="C161" t="n">
-        <v>0.37615357518452974</v>
+        <v>0.37527746383537003</v>
       </c>
       <c r="D161" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C162" t="n">
-        <v>0.1410652520613998</v>
+        <v>0.3825159409815373</v>
       </c>
       <c r="D162" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B163" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1024251835908396</v>
+        <v>0.3953338772612408</v>
       </c>
       <c r="D163" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B164" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C164" t="n">
-        <v>0.38468272501345163</v>
+        <v>0.15761636258407077</v>
       </c>
       <c r="D164" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B165" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C165" t="n">
-        <v>0.15841345977590288</v>
+        <v>0.3988193534146727</v>
       </c>
       <c r="D165" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C166" t="n">
-        <v>0.3957061533717947</v>
+        <v>0.33030736573320657</v>
       </c>
       <c r="D166" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="B167" t="s">
         <v>5</v>
       </c>
       <c r="C167" t="n">
-        <v>0.3408823498110449</v>
+        <v>0.36817110912286477</v>
       </c>
       <c r="D167" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B168" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C168" t="n">
-        <v>0.1419411656589489</v>
+        <v>0.3985764812826302</v>
       </c>
       <c r="D168" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
       <c r="B169" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C169" t="n">
-        <v>0.33732960786966026</v>
+        <v>0.21688642977543254</v>
       </c>
       <c r="D169" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
       </c>
       <c r="C170" t="n">
-        <v>0.08913940893535027</v>
+        <v>0.15415509696374408</v>
       </c>
       <c r="D170" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B171" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C171" t="n">
-        <v>0.35266867189117745</v>
+        <v>0.3505871320143275</v>
       </c>
       <c r="D171" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>164</v>
+        <v>46</v>
       </c>
       <c r="B172" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C172" t="n">
-        <v>0.13079041473158398</v>
+        <v>0.3860850272589179</v>
       </c>
       <c r="D172" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B173" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C173" t="n">
-        <v>0.15833022759860066</v>
+        <v>0.3989420726070041</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B174" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C174" t="n">
-        <v>0.34109581055458865</v>
+        <v>0.266247959980625</v>
       </c>
       <c r="D174" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B175" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C175" t="n">
-        <v>0.3938848377602154</v>
+        <v>0.053967028268770305</v>
       </c>
       <c r="D175" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B176" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C176" t="n">
-        <v>0.024375451233784803</v>
+        <v>0.394953303746838</v>
       </c>
       <c r="D176" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="B177" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C177" t="n">
-        <v>0.2748343890926546</v>
+        <v>0.38528417831985695</v>
       </c>
       <c r="D177" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B178" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C178" t="n">
-        <v>0.37749041399118927</v>
+        <v>0.2172316460266999</v>
       </c>
       <c r="D178" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B179" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C179" t="n">
-        <v>0.38217542186347697</v>
+        <v>0.396728336774955</v>
       </c>
       <c r="D179" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B180" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C180" t="n">
-        <v>0.221166757240653</v>
+        <v>0.25582560639082746</v>
       </c>
       <c r="D180" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B181" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C181" t="n">
-        <v>0.2659021714911606</v>
+        <v>0.3365892951846078</v>
       </c>
       <c r="D181" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generator updated to run CSVFileReader methods
</commit_message>
<xml_diff>
--- a/Analysis120.xlsx
+++ b/Analysis120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="177">
   <si>
     <t>Research Activity</t>
   </si>
@@ -26,517 +26,523 @@
     <t>Percentage Distribution</t>
   </si>
   <si>
-    <t>suing large corporations</t>
+    <t>nurturing sibling rivalry</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>1.08%</t>
+  </si>
+  <si>
+    <t>hunting serial killers</t>
+  </si>
+  <si>
+    <t>1.17%</t>
+  </si>
+  <si>
+    <t>singing punk rock songs</t>
   </si>
   <si>
     <t>CS+DS</t>
   </si>
   <si>
+    <t>0.50%</t>
+  </si>
+  <si>
+    <t>piloting a spaceship</t>
+  </si>
+  <si>
+    <t>0.83%</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
+  </si>
+  <si>
+    <t>0.33%</t>
+  </si>
+  <si>
+    <t>practicing insincerity</t>
+  </si>
+  <si>
+    <t>0.75%</t>
+  </si>
+  <si>
+    <t>scandalizing polite society</t>
+  </si>
+  <si>
+    <t>painting dark pictures</t>
+  </si>
+  <si>
+    <t>0.25%</t>
+  </si>
+  <si>
+    <t>adopting children</t>
+  </si>
+  <si>
+    <t>0.17%</t>
+  </si>
+  <si>
+    <t>picking pockets</t>
+  </si>
+  <si>
+    <t>running an empire</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>moaning about men</t>
+  </si>
+  <si>
+    <t>fighting civil wars</t>
+  </si>
+  <si>
+    <t>singing torch songs</t>
+  </si>
+  <si>
+    <t>gyrating hips</t>
+  </si>
+  <si>
+    <t>0.42%</t>
+  </si>
+  <si>
+    <t>making witty remarks</t>
+  </si>
+  <si>
+    <t>giving investment advice</t>
+  </si>
+  <si>
+    <t>0.58%</t>
+  </si>
+  <si>
+    <t>modeling clothes</t>
+  </si>
+  <si>
+    <t>studying gorillas up close</t>
+  </si>
+  <si>
+    <t>solving mysteries</t>
+  </si>
+  <si>
+    <t>writing on wax tablets</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>fighting for justice</t>
+  </si>
+  <si>
+    <t>brokering peace deals</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies</t>
+  </si>
+  <si>
+    <t>0.08%</t>
+  </si>
+  <si>
+    <t>winning Oscars</t>
+  </si>
+  <si>
+    <t>defending the weak</t>
+  </si>
+  <si>
+    <t>0.67%</t>
+  </si>
+  <si>
+    <t>throwing lavish parties</t>
+  </si>
+  <si>
+    <t>eating carrots</t>
+  </si>
+  <si>
+    <t>spying for the CIA</t>
+  </si>
+  <si>
+    <t>starring in daytime soap operas</t>
+  </si>
+  <si>
+    <t>campaigning for social causes</t>
+  </si>
+  <si>
+    <t>posing for photographs</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
+  </si>
+  <si>
+    <t>making provocative documentaries</t>
+  </si>
+  <si>
+    <t>walking like a man</t>
+  </si>
+  <si>
+    <t>avoiding paparazzi</t>
+  </si>
+  <si>
+    <t>hacking into corporate mainframes</t>
+  </si>
+  <si>
+    <t>making suspense movies</t>
+  </si>
+  <si>
+    <t>getting plastic surgery</t>
+  </si>
+  <si>
+    <t>drinking too much red wine</t>
+  </si>
+  <si>
+    <t>starring in sit-coms</t>
+  </si>
+  <si>
+    <t>solving crimes</t>
+  </si>
+  <si>
+    <t>selling chrystal meth</t>
+  </si>
+  <si>
+    <t>complaining about everything</t>
+  </si>
+  <si>
+    <t>1.42%</t>
+  </si>
+  <si>
+    <t>designing modern buildings</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes</t>
+  </si>
+  <si>
+    <t>hosting reality TV shows</t>
+  </si>
+  <si>
+    <t>commanding a spaceship</t>
+  </si>
+  <si>
+    <t>writing short stories</t>
+  </si>
+  <si>
+    <t>making unauthorized sex tapes</t>
+  </si>
+  <si>
+    <t>seducing young women</t>
+  </si>
+  <si>
+    <t>chasing interns</t>
+  </si>
+  <si>
+    <t>pulling dirty political tricks</t>
+  </si>
+  <si>
+    <t>collecting treasures</t>
+  </si>
+  <si>
+    <t>fighting for democracy</t>
+  </si>
+  <si>
+    <t>building empires</t>
+  </si>
+  <si>
+    <t>making new wave movies</t>
+  </si>
+  <si>
+    <t>mangling idioms</t>
+  </si>
+  <si>
+    <t>promoting conservative values</t>
+  </si>
+  <si>
+    <t>racking up marriages</t>
+  </si>
+  <si>
+    <t>writing plays about the middle classes</t>
+  </si>
+  <si>
     <t>0.92%</t>
   </si>
   <si>
-    <t>starring in romantic comedies</t>
-  </si>
-  <si>
-    <t>0.67%</t>
-  </si>
-  <si>
-    <t>writing pop songs</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>0.50%</t>
-  </si>
-  <si>
-    <t>writing beat fiction</t>
-  </si>
-  <si>
-    <t>creating monsters</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>solving mysteries</t>
-  </si>
-  <si>
-    <t>0.25%</t>
-  </si>
-  <si>
-    <t>singing blues songs</t>
-  </si>
-  <si>
-    <t>0.75%</t>
-  </si>
-  <si>
-    <t>writing TV comedies</t>
-  </si>
-  <si>
-    <t>0.08%</t>
-  </si>
-  <si>
-    <t>preaching to presidents</t>
-  </si>
-  <si>
-    <t>0.83%</t>
-  </si>
-  <si>
-    <t>interviewing politicians</t>
-  </si>
-  <si>
-    <t>0.42%</t>
-  </si>
-  <si>
-    <t>running a school for gifted teens</t>
+    <t>buying on credit</t>
+  </si>
+  <si>
+    <t>climbing social ladders</t>
+  </si>
+  <si>
+    <t>trading innuendo</t>
+  </si>
+  <si>
+    <t>ranting about liberals</t>
+  </si>
+  <si>
+    <t>currying favour</t>
+  </si>
+  <si>
+    <t>running a criminal enterprise</t>
+  </si>
+  <si>
+    <t>1.25%</t>
+  </si>
+  <si>
+    <t>running a multinational corporation</t>
+  </si>
+  <si>
+    <t>preventing crime</t>
+  </si>
+  <si>
+    <t>promoting communism</t>
+  </si>
+  <si>
+    <t>pedalling furiously</t>
+  </si>
+  <si>
+    <t>singing rock songs</t>
+  </si>
+  <si>
+    <t>writing modern fiction</t>
+  </si>
+  <si>
+    <t>organizing armed robberies</t>
+  </si>
+  <si>
+    <t>developing advertising campaigns</t>
+  </si>
+  <si>
+    <t>solving riddles</t>
+  </si>
+  <si>
+    <t>impersonating women</t>
+  </si>
+  <si>
+    <t>singing country music</t>
+  </si>
+  <si>
+    <t>spreading revolution</t>
+  </si>
+  <si>
+    <t>signing sports memorabilia</t>
+  </si>
+  <si>
+    <t>living amongst apes</t>
+  </si>
+  <si>
+    <t>selling cheap airline seats</t>
+  </si>
+  <si>
+    <t>delivering presents</t>
+  </si>
+  <si>
+    <t>playing everyman characters</t>
+  </si>
+  <si>
+    <t>promoting logical thinking</t>
+  </si>
+  <si>
+    <t>foiling the schemes of evil villains</t>
+  </si>
+  <si>
+    <t>stealing jewels</t>
+  </si>
+  <si>
+    <t>developing new technologies</t>
+  </si>
+  <si>
+    <t>rescuing hostages</t>
+  </si>
+  <si>
+    <t>1.00%</t>
+  </si>
+  <si>
+    <t>flirting with rednecks</t>
+  </si>
+  <si>
+    <t>promoting hair products</t>
+  </si>
+  <si>
+    <t>promoting big business</t>
+  </si>
+  <si>
+    <t>disposing of unwanted jewelry</t>
+  </si>
+  <si>
+    <t>managing large development projects</t>
+  </si>
+  <si>
+    <t>bullying schoolkids</t>
+  </si>
+  <si>
+    <t>smoking Laramie Hi-Tars</t>
+  </si>
+  <si>
+    <t>developing military strategies</t>
+  </si>
+  <si>
+    <t>clipping coupons</t>
+  </si>
+  <si>
+    <t>painting abstract pictures</t>
+  </si>
+  <si>
+    <t>speaking with funny accents</t>
+  </si>
+  <si>
+    <t>playing soccer</t>
+  </si>
+  <si>
+    <t>ruling over subjects</t>
+  </si>
+  <si>
+    <t>pretending to wrestle</t>
+  </si>
+  <si>
+    <t>analyzing the sub-conscious</t>
+  </si>
+  <si>
+    <t>peacocking in fancy clothes</t>
+  </si>
+  <si>
+    <t>starring in comedies</t>
+  </si>
+  <si>
+    <t>reporting the news</t>
+  </si>
+  <si>
+    <t>writing plays</t>
+  </si>
+  <si>
+    <t>writing purple prose</t>
+  </si>
+  <si>
+    <t>ranting about politics</t>
+  </si>
+  <si>
+    <t>promoting openness</t>
+  </si>
+  <si>
+    <t>playing baseball</t>
+  </si>
+  <si>
+    <t>writing crime stories</t>
+  </si>
+  <si>
+    <t>burning the wicked</t>
+  </si>
+  <si>
+    <t>racing fast cars</t>
   </si>
   <si>
     <t>playing aggressive chess</t>
   </si>
   <si>
-    <t>0.33%</t>
+    <t>performing magic tricks</t>
+  </si>
+  <si>
+    <t>seeking revenge</t>
+  </si>
+  <si>
+    <t>running races</t>
+  </si>
+  <si>
+    <t>raising a family</t>
+  </si>
+  <si>
+    <t>smoking during recess</t>
+  </si>
+  <si>
+    <t>terrorizing prostitutes</t>
+  </si>
+  <si>
+    <t>promoting the Web</t>
+  </si>
+  <si>
+    <t>cooking dinners</t>
+  </si>
+  <si>
+    <t>commanding a whaling ship</t>
+  </si>
+  <si>
+    <t>fomenting social revolution</t>
+  </si>
+  <si>
+    <t>singing romantic songs</t>
+  </si>
+  <si>
+    <t>interviewing celebrities</t>
+  </si>
+  <si>
+    <t>making home-made clothes</t>
+  </si>
+  <si>
+    <t>1.33%</t>
+  </si>
+  <si>
+    <t>running the FBI</t>
+  </si>
+  <si>
+    <t>winning tennis matches</t>
+  </si>
+  <si>
+    <t>killing demons</t>
+  </si>
+  <si>
+    <t>starring in reality TV shows</t>
+  </si>
+  <si>
+    <t>chasing murderers</t>
+  </si>
+  <si>
+    <t>commiting perjury</t>
+  </si>
+  <si>
+    <t>posing riddles</t>
+  </si>
+  <si>
+    <t>looking for hidden treasures</t>
+  </si>
+  <si>
+    <t>singing experimental songs</t>
+  </si>
+  <si>
+    <t>stabbing in the back</t>
+  </si>
+  <si>
+    <t>writing poetry</t>
+  </si>
+  <si>
+    <t>attending cocktail parties</t>
+  </si>
+  <si>
+    <t>digging for antiquities</t>
+  </si>
+  <si>
+    <t>staring at the moon</t>
+  </si>
+  <si>
+    <t>knocking out opponents</t>
+  </si>
+  <si>
+    <t>publishing newspapers</t>
+  </si>
+  <si>
+    <t>teaching the next generation</t>
+  </si>
+  <si>
+    <t>pulling capers</t>
   </si>
   <si>
     <t>starring in pornographic movies</t>
   </si>
   <si>
-    <t>0.17%</t>
-  </si>
-  <si>
-    <t>spreading revolution</t>
-  </si>
-  <si>
-    <t>campaigning for social causes</t>
-  </si>
-  <si>
-    <t>starring in madcap comedies</t>
-  </si>
-  <si>
-    <t>studying gorillas up close</t>
-  </si>
-  <si>
-    <t>telling epic tales</t>
-  </si>
-  <si>
-    <t>assassinating presidents</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>0.58%</t>
-  </si>
-  <si>
-    <t>promoting Catholic values</t>
-  </si>
-  <si>
-    <t>posing for photographs</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
-    <t>flaunting foppish fashions</t>
-  </si>
-  <si>
-    <t>making billions</t>
-  </si>
-  <si>
-    <t>playing the saxophone</t>
-  </si>
-  <si>
-    <t>starring in TV shows</t>
-  </si>
-  <si>
-    <t>pioneering new technologies</t>
-  </si>
-  <si>
-    <t>teaching the next generation</t>
-  </si>
-  <si>
-    <t>making unauthorized sex tapes</t>
-  </si>
-  <si>
-    <t>singing opera arias</t>
-  </si>
-  <si>
-    <t>1.00%</t>
-  </si>
-  <si>
-    <t>writing modern poetry</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes</t>
-  </si>
-  <si>
-    <t>telling dry jokes</t>
-  </si>
-  <si>
-    <t>winning battles</t>
-  </si>
-  <si>
-    <t>defending plaintiffs</t>
-  </si>
-  <si>
-    <t>running a tech giant</t>
-  </si>
-  <si>
-    <t>trading in wives</t>
-  </si>
-  <si>
-    <t>inventing electrical marvels</t>
-  </si>
-  <si>
-    <t>running an empire</t>
-  </si>
-  <si>
-    <t>singing pop songs</t>
-  </si>
-  <si>
-    <t>keeping a diary</t>
-  </si>
-  <si>
-    <t>singing melancholy songs</t>
-  </si>
-  <si>
-    <t>brokering peace deals</t>
-  </si>
-  <si>
-    <t>warning about totalitarianism</t>
-  </si>
-  <si>
-    <t>promoting greed</t>
-  </si>
-  <si>
-    <t>fighting civil wars</t>
-  </si>
-  <si>
-    <t>grabbing power</t>
-  </si>
-  <si>
-    <t>hiding from the public</t>
-  </si>
-  <si>
-    <t>clipping coupons</t>
-  </si>
-  <si>
-    <t>enriching uranium</t>
-  </si>
-  <si>
-    <t>dripping paint onto canvas</t>
-  </si>
-  <si>
-    <t>selling comic books</t>
-  </si>
-  <si>
-    <t>fighting the resistance</t>
-  </si>
-  <si>
-    <t>1.17%</t>
-  </si>
-  <si>
-    <t>suppressing violent urges</t>
-  </si>
-  <si>
-    <t>playing rock guitar</t>
-  </si>
-  <si>
-    <t>losing control</t>
-  </si>
-  <si>
-    <t>1.25%</t>
-  </si>
-  <si>
-    <t>fighting for civil rights</t>
-  </si>
-  <si>
-    <t>picking pockets</t>
-  </si>
-  <si>
-    <t>winning Michelin stars</t>
-  </si>
-  <si>
-    <t>making dunk shots</t>
-  </si>
-  <si>
-    <t>selling perfumes</t>
-  </si>
-  <si>
-    <t>planting daffodils</t>
-  </si>
-  <si>
-    <t>1.33%</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies</t>
-  </si>
-  <si>
-    <t>singing Hipbop songs</t>
-  </si>
-  <si>
-    <t>gossiping with galpals</t>
-  </si>
-  <si>
-    <t>1.08%</t>
-  </si>
-  <si>
-    <t>making vulgar jokes</t>
-  </si>
-  <si>
-    <t>starring in comedies</t>
-  </si>
-  <si>
-    <t>competing in the Olympics</t>
-  </si>
-  <si>
-    <t>doing stand-up</t>
-  </si>
-  <si>
-    <t>promoting communism</t>
-  </si>
-  <si>
-    <t>writing experimental songs</t>
-  </si>
-  <si>
-    <t>causing mayhem</t>
-  </si>
-  <si>
-    <t>playing soccer</t>
-  </si>
-  <si>
-    <t>writing epic poetry</t>
-  </si>
-  <si>
-    <t>forging art</t>
-  </si>
-  <si>
-    <t>running a crime family</t>
-  </si>
-  <si>
-    <t>plotting strategies</t>
-  </si>
-  <si>
-    <t>ranting about politics</t>
-  </si>
-  <si>
-    <t>offering advice</t>
-  </si>
-  <si>
-    <t>manipulating political pawns</t>
-  </si>
-  <si>
-    <t>living amongst apes</t>
-  </si>
-  <si>
-    <t>turning it up to 11</t>
-  </si>
-  <si>
-    <t>playing God</t>
-  </si>
-  <si>
-    <t>climbing down chimneys</t>
-  </si>
-  <si>
-    <t>winning swimming competitions</t>
-  </si>
-  <si>
-    <t>arresting bootleggers</t>
-  </si>
-  <si>
-    <t>making strategic decisions</t>
-  </si>
-  <si>
-    <t>studying magic tricks</t>
-  </si>
-  <si>
-    <t>running film festivals</t>
-  </si>
-  <si>
-    <t>solving riddles</t>
-  </si>
-  <si>
-    <t>losing court cases</t>
-  </si>
-  <si>
-    <t>running theme parks</t>
-  </si>
-  <si>
-    <t>throwing fund-raisers for Parkinson's disease</t>
-  </si>
-  <si>
-    <t>commanding a spaceship</t>
-  </si>
-  <si>
-    <t>searching for the messiah</t>
-  </si>
-  <si>
-    <t>1.42%</t>
-  </si>
-  <si>
-    <t>exploring darkest Africa</t>
-  </si>
-  <si>
-    <t>collecting rock samples</t>
-  </si>
-  <si>
-    <t>avoiding growing old</t>
-  </si>
-  <si>
-    <t>singing parody songs</t>
-  </si>
-  <si>
-    <t>duelling acrobatically</t>
-  </si>
-  <si>
-    <t>writing plays about the middle classes</t>
-  </si>
-  <si>
-    <t>spying for the enemy</t>
-  </si>
-  <si>
-    <t>winning boxing matches</t>
-  </si>
-  <si>
-    <t>battling the forces of darkness</t>
-  </si>
-  <si>
-    <t>creating dictionaries</t>
-  </si>
-  <si>
-    <t>studying science</t>
-  </si>
-  <si>
-    <t>cleaning floors</t>
-  </si>
-  <si>
-    <t>climbing social ladders</t>
-  </si>
-  <si>
-    <t>seducing women</t>
-  </si>
-  <si>
-    <t>doing raunchy stage acts</t>
-  </si>
-  <si>
-    <t>looking after children</t>
-  </si>
-  <si>
-    <t>seducing young women</t>
-  </si>
-  <si>
-    <t>writing erotic fiction</t>
-  </si>
-  <si>
-    <t>walking like a man</t>
-  </si>
-  <si>
-    <t>finding clues</t>
-  </si>
-  <si>
-    <t>developing military strategies</t>
-  </si>
-  <si>
-    <t>abusing power</t>
-  </si>
-  <si>
-    <t>instigating rebellion</t>
-  </si>
-  <si>
-    <t>running a frontier town</t>
-  </si>
-  <si>
-    <t>campaigning for democracy</t>
-  </si>
-  <si>
-    <t>setting mousetraps</t>
-  </si>
-  <si>
-    <t>writing funny movies</t>
-  </si>
-  <si>
-    <t>directing the business of state</t>
-  </si>
-  <si>
-    <t>analyzing the sub-conscious</t>
-  </si>
-  <si>
-    <t>spreading political gossip</t>
-  </si>
-  <si>
-    <t>fussing about cleanliness</t>
-  </si>
-  <si>
-    <t>pursuing criminals</t>
-  </si>
-  <si>
-    <t>directing animated films</t>
-  </si>
-  <si>
-    <t>promoting pop music</t>
-  </si>
-  <si>
-    <t>preparing for the apocalypse</t>
-  </si>
-  <si>
-    <t>telling tall tales</t>
-  </si>
-  <si>
-    <t>manipulating ingenues</t>
-  </si>
-  <si>
-    <t>cheating at poker</t>
-  </si>
-  <si>
-    <t>selling airline seats</t>
-  </si>
-  <si>
-    <t>peacocking in fancy clothes</t>
-  </si>
-  <si>
-    <t>playing James Bond</t>
-  </si>
-  <si>
-    <t>running a business empire</t>
-  </si>
-  <si>
-    <t>fighting with the mob</t>
-  </si>
-  <si>
-    <t>guarding the galaxy</t>
-  </si>
-  <si>
-    <t>fighting with swords</t>
-  </si>
-  <si>
-    <t>exorcising demons</t>
-  </si>
-  <si>
-    <t>issuing fatwas</t>
-  </si>
-  <si>
-    <t>promoting racial harmony</t>
-  </si>
-  <si>
-    <t>preaching tolerance</t>
-  </si>
-  <si>
-    <t>playing the organ</t>
-  </si>
-  <si>
-    <t>moaning about men</t>
-  </si>
-  <si>
-    <t>falling in love</t>
-  </si>
-  <si>
-    <t>avenging loved ones</t>
-  </si>
-  <si>
-    <t>counting tooth picks</t>
-  </si>
-  <si>
-    <t>exploring foreign countries</t>
+    <t>building giant walls</t>
+  </si>
+  <si>
+    <t>phoning home</t>
+  </si>
+  <si>
+    <t>selling consumer goods</t>
+  </si>
+  <si>
+    <t>hunting raccoons</t>
   </si>
 </sst>
 </file>
@@ -594,7 +600,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="37.46875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="31.71875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.11328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.671875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="27.51953125" customWidth="true" bestFit="true"/>
@@ -622,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3771525118200255</v>
+        <v>0.3532422469981089</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -636,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3646255019797833</v>
+        <v>0.23209711804470248</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -650,7 +656,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0.255604520663135</v>
+        <v>0.18867751387617682</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -661,55 +667,55 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.39855096910266485</v>
+        <v>0.2535506343627881</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>0.388105506826859</v>
+        <v>0.20888337013004524</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.09675692324692625</v>
+        <v>0.2739982845466959</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>0.37411378586688787</v>
+        <v>0.20614851337054893</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -717,10 +723,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>0.12758496465270888</v>
+        <v>0.381197722310815</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -731,10 +737,10 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3926282967706807</v>
+        <v>0.17217915351424268</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -745,27 +751,27 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1500881269848936</v>
+        <v>0.32657653888869276</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C12" t="n">
-        <v>0.22290217075841404</v>
+        <v>0.23333760728440833</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -776,122 +782,122 @@
         <v>10</v>
       </c>
       <c r="C13" t="n">
-        <v>0.38501546614117244</v>
+        <v>0.1770619624557211</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>0.09671525303963519</v>
+        <v>0.24033918374289504</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C15" t="n">
-        <v>0.39350458851137604</v>
+        <v>0.3515258486485477</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2815999764677612</v>
+        <v>0.3385814770865572</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C17" t="n">
-        <v>0.39850952592190614</v>
+        <v>0.19881108744266796</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1700007606877913</v>
+        <v>0.3953530503101488</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C19" t="n">
-        <v>0.09147267907267095</v>
+        <v>0.3558309385610985</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C20" t="n">
-        <v>0.14788062035783547</v>
+        <v>0.10955104059093469</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>0.38112907723153805</v>
+        <v>0.0991054640178778</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -899,517 +905,517 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3750041096359953</v>
+        <v>0.18376186112039597</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0345635701188219</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.29165648462817423</v>
-      </c>
-      <c r="D23" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="n">
-        <v>0.007791466886580667</v>
+        <v>0.3988652493431996</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>0.21703594955967992</v>
+        <v>0.39832260315975415</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.3149894115271835</v>
+        <v>0.2691430963611282</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0751743744798041</v>
+      </c>
+      <c r="D27" t="s">
         <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.36087195461953875</v>
-      </c>
-      <c r="D27" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C28" t="n">
-        <v>0.39852341427127824</v>
+        <v>0.3668896021957355</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="n">
-        <v>0.3988341899937757</v>
+        <v>0.2567602935414122</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3579884829480844</v>
+        <v>0.3543466068585939</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>0.27621421844493715</v>
+        <v>0.22088657772518153</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C32" t="n">
-        <v>0.39257258315500143</v>
+        <v>0.22845724547528978</v>
       </c>
       <c r="D32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>0.3903961138515097</v>
+        <v>0.03120319909920744</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C34" t="n">
-        <v>0.37158550587196204</v>
+        <v>0.3979716638272976</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C35" t="n">
-        <v>0.39609459835435085</v>
+        <v>0.2713383579767237</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C36" t="n">
-        <v>0.26105776079742954</v>
+        <v>0.3795569486990401</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C37" t="n">
-        <v>0.052344178983057384</v>
+        <v>0.3953957849651966</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
       </c>
       <c r="C38" t="n">
-        <v>0.16007345584935626</v>
+        <v>0.39227858822785494</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>0.23491068183550962</v>
+        <v>0.3810468387699379</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="n">
-        <v>0.3438042307426023</v>
+        <v>0.21150435477583013</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
       </c>
       <c r="C41" t="n">
-        <v>0.11635006788537892</v>
+        <v>0.3205722337608767</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C42" t="n">
-        <v>0.35460801021166716</v>
+        <v>0.3137713967462525</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>0.12951637466057678</v>
+        <v>0.3607407305509403</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C44" t="n">
-        <v>0.30702363753132356</v>
+        <v>0.3383450360047825</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2948680118341556</v>
+        <v>0.25305617839378225</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
       </c>
       <c r="C46" t="n">
-        <v>0.16421422967457672</v>
+        <v>0.11549407034111454</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.360713655672053</v>
+        <v>0.09551074746942431</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.10313488311457508</v>
+        <v>0.39890440824177903</v>
       </c>
       <c r="D48" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2504716916054045</v>
+        <v>0.39675854319394277</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C50" t="n">
-        <v>0.11760559881202408</v>
+        <v>0.33099717752714036</v>
       </c>
       <c r="D50" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>0.008079313274094096</v>
+        <v>0.12940111164611998</v>
       </c>
       <c r="D51" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>0.3943773182159054</v>
+        <v>0.3284835907719739</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C53" t="n">
-        <v>0.23321148571638758</v>
+        <v>0.09776533205881296</v>
       </c>
       <c r="D53" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C54" t="n">
-        <v>0.15169143052674494</v>
+        <v>0.34524289736330593</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1522172195863736</v>
+        <v>0.13179058278791153</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C56" t="n">
-        <v>0.3260413761879838</v>
+        <v>0.03483889033611339</v>
       </c>
       <c r="D56" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>0.2927306117747792</v>
+        <v>0.2580070060576051</v>
       </c>
       <c r="D57" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C58" t="n">
-        <v>0.3707107397019012</v>
+        <v>0.270439307282296</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59">
@@ -1417,13 +1423,13 @@
         <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>0.03780251639704063</v>
+        <v>0.3900089953340393</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60">
@@ -1431,13 +1437,13 @@
         <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C60" t="n">
-        <v>0.04258837114393448</v>
+        <v>0.13203185594045783</v>
       </c>
       <c r="D60" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61">
@@ -1445,24 +1451,24 @@
         <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C61" t="n">
-        <v>0.3910241760657666</v>
+        <v>0.1983577739657499</v>
       </c>
       <c r="D61" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C62" t="n">
-        <v>0.11930650046219593</v>
+        <v>0.32787293833772774</v>
       </c>
       <c r="D62" t="s">
         <v>20</v>
@@ -1470,58 +1476,58 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>0.35064425483769696</v>
+        <v>0.3965439885422644</v>
       </c>
       <c r="D63" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
       </c>
       <c r="C64" t="n">
-        <v>0.19220817712851088</v>
+        <v>0.23265558043605356</v>
       </c>
       <c r="D64" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3030941823190015</v>
+        <v>0.3886537772831908</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C66" t="n">
-        <v>0.2797147654195351</v>
+        <v>0.09906674253994216</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67">
@@ -1529,80 +1535,80 @@
         <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C67" t="n">
-        <v>0.12931253220924038</v>
+        <v>0.37546441343926884</v>
       </c>
       <c r="D67" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" t="n">
-        <v>0.20633838793970785</v>
+        <v>0.39291711192647016</v>
       </c>
       <c r="D68" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C69" t="n">
-        <v>0.37704895531483745</v>
+        <v>0.2773408038366134</v>
       </c>
       <c r="D69" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C70" t="n">
-        <v>0.3526339359971409</v>
+        <v>0.3375256534056661</v>
       </c>
       <c r="D70" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
       </c>
       <c r="C71" t="n">
-        <v>0.39014248126527284</v>
+        <v>0.18105196667024062</v>
       </c>
       <c r="D71" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C72" t="n">
-        <v>0.2230534173834142</v>
+        <v>0.34723063878229027</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
@@ -1610,419 +1616,419 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C73" t="n">
-        <v>0.3545240444591294</v>
+        <v>0.39374534969493163</v>
       </c>
       <c r="D73" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C74" t="n">
-        <v>0.27018722764482594</v>
+        <v>0.39744310645998154</v>
       </c>
       <c r="D74" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C75" t="n">
-        <v>0.21586387809319296</v>
+        <v>0.16667286643010942</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
       <c r="C76" t="n">
-        <v>0.3674665698368085</v>
+        <v>0.31164684138605664</v>
       </c>
       <c r="D76" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3697159583114312</v>
+        <v>0.355905558678136</v>
       </c>
       <c r="D77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C78" t="n">
-        <v>0.16683323785450918</v>
+        <v>0.3418316767623597</v>
       </c>
       <c r="D78" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C79" t="n">
-        <v>0.2583412038093409</v>
+        <v>0.34014745326715806</v>
       </c>
       <c r="D79" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" t="n">
-        <v>0.387729515692608</v>
+        <v>0.39556941588450373</v>
       </c>
       <c r="D80" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>0.39839934009451644</v>
+        <v>0.38754197873700436</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C82" t="n">
-        <v>0.12637977946021792</v>
+        <v>0.3957775613987749</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B83" t="s">
         <v>10</v>
       </c>
       <c r="C83" t="n">
-        <v>0.16393244269134918</v>
+        <v>0.3821139891082932</v>
       </c>
       <c r="D83" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.36043939674392395</v>
+      </c>
+      <c r="D84" t="s">
         <v>15</v>
-      </c>
-      <c r="B84" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" t="n">
-        <v>0.37904591389936687</v>
-      </c>
-      <c r="D84" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C85" t="n">
-        <v>0.3974562484797686</v>
+        <v>0.14203647793855803</v>
       </c>
       <c r="D85" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C86" t="n">
-        <v>0.11193857033695064</v>
+        <v>0.2843317423091485</v>
       </c>
       <c r="D86" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
       <c r="C87" t="n">
-        <v>0.39464737901511876</v>
+        <v>0.1431661212846734</v>
       </c>
       <c r="D87" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C88" t="n">
-        <v>0.21962218538002148</v>
+        <v>0.3822048218078074</v>
       </c>
       <c r="D88" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C89" t="n">
-        <v>0.3326842355438256</v>
+        <v>0.3325406412974541</v>
       </c>
       <c r="D89" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1932607567866209</v>
+        <v>0.33384735365248586</v>
       </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>0.24743536451615375</v>
+        <v>0.01388788342892639</v>
       </c>
       <c r="D91" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
       </c>
       <c r="C92" t="n">
-        <v>0.36823729671489497</v>
+        <v>0.24492786807313766</v>
       </c>
       <c r="D92" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C93" t="n">
-        <v>0.07070116960420744</v>
+        <v>0.2560189839897271</v>
       </c>
       <c r="D93" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B94" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C94" t="n">
-        <v>0.3986312601205356</v>
+        <v>0.3722562175799145</v>
       </c>
       <c r="D94" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1738155154936748</v>
+        <v>0.3136044842359758</v>
       </c>
       <c r="D95" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C96" t="n">
-        <v>0.3864857911832088</v>
+        <v>0.24978928888187565</v>
       </c>
       <c r="D96" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B97" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C97" t="n">
-        <v>0.3203700060056968</v>
+        <v>0.15354661700123257</v>
       </c>
       <c r="D97" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
         <v>5</v>
       </c>
       <c r="C98" t="n">
-        <v>0.21557862302049197</v>
+        <v>0.11689595594781996</v>
       </c>
       <c r="D98" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B99" t="s">
         <v>5</v>
       </c>
       <c r="C99" t="n">
-        <v>0.09365391903615662</v>
+        <v>0.3807739626526599</v>
       </c>
       <c r="D99" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
       </c>
       <c r="C100" t="n">
-        <v>0.3912132765051571</v>
+        <v>0.3860214559224575</v>
       </c>
       <c r="D100" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C101" t="n">
-        <v>0.3673221310241492</v>
+        <v>0.15222564238235484</v>
       </c>
       <c r="D101" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B102" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C102" t="n">
-        <v>0.3474446539937292</v>
+        <v>0.34637491522305325</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
@@ -2030,16 +2036,16 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.39592408675227303</v>
+      </c>
+      <c r="D103" t="s">
         <v>112</v>
-      </c>
-      <c r="B103" t="s">
-        <v>10</v>
-      </c>
-      <c r="C103" t="n">
-        <v>0.12902478428653474</v>
-      </c>
-      <c r="D103" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="104">
@@ -2047,195 +2053,195 @@
         <v>113</v>
       </c>
       <c r="B104" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C104" t="n">
-        <v>0.3466071608131492</v>
+        <v>0.04727455740097066</v>
       </c>
       <c r="D104" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
       </c>
       <c r="C105" t="n">
-        <v>0.3966350569353832</v>
+        <v>0.3149991515129434</v>
       </c>
       <c r="D105" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C106" t="n">
-        <v>0.31534200744168117</v>
+        <v>0.27919923538513364</v>
       </c>
       <c r="D106" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="B107" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C107" t="n">
-        <v>0.2927572815908294</v>
+        <v>0.17235862562875445</v>
       </c>
       <c r="D107" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C108" t="n">
-        <v>0.16223763462710555</v>
+        <v>0.3984750594634033</v>
       </c>
       <c r="D108" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B109" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1887011488739992</v>
+        <v>0.12713013974257972</v>
       </c>
       <c r="D109" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C110" t="n">
-        <v>0.26507535903354684</v>
+        <v>0.39728044359510845</v>
       </c>
       <c r="D110" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B111" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C111" t="n">
-        <v>0.152007053310442</v>
+        <v>0.39339814332501244</v>
       </c>
       <c r="D111" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B112" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C112" t="n">
-        <v>0.34861892203892547</v>
+        <v>0.3703530922204387</v>
       </c>
       <c r="D112" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C113" t="n">
-        <v>0.3979525123671936</v>
+        <v>0.37911410284575214</v>
       </c>
       <c r="D113" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C114" t="n">
-        <v>0.23263872870350708</v>
+        <v>0.3309763030031872</v>
       </c>
       <c r="D114" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="B115" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1284531072635669</v>
+        <v>0.3289936042083508</v>
       </c>
       <c r="D115" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C116" t="n">
-        <v>0.16251453160036733</v>
+        <v>0.39829072836212615</v>
       </c>
       <c r="D116" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B117" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C117" t="n">
-        <v>0.20316774526260142</v>
+        <v>0.16298967699467137</v>
       </c>
       <c r="D117" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118">
@@ -2243,13 +2249,13 @@
         <v>125</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C118" t="n">
-        <v>0.3458699515754768</v>
+        <v>0.37007335914245443</v>
       </c>
       <c r="D118" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119">
@@ -2257,13 +2263,13 @@
         <v>126</v>
       </c>
       <c r="B119" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C119" t="n">
-        <v>0.3946435663698323</v>
+        <v>0.20552047815385113</v>
       </c>
       <c r="D119" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120">
@@ -2271,13 +2277,13 @@
         <v>127</v>
       </c>
       <c r="B120" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C120" t="n">
-        <v>0.39828653159282507</v>
+        <v>0.16323316812755184</v>
       </c>
       <c r="D120" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121">
@@ -2285,10 +2291,10 @@
         <v>128</v>
       </c>
       <c r="B121" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C121" t="n">
-        <v>0.11324385868196526</v>
+        <v>0.20201407607085217</v>
       </c>
       <c r="D121" t="s">
         <v>11</v>
@@ -2299,13 +2305,13 @@
         <v>129</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C122" t="n">
-        <v>0.3482862173983848</v>
+        <v>0.27332077378628433</v>
       </c>
       <c r="D122" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123">
@@ -2313,13 +2319,13 @@
         <v>130</v>
       </c>
       <c r="B123" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C123" t="n">
-        <v>0.06573755020454998</v>
+        <v>0.2982225548321427</v>
       </c>
       <c r="D123" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124">
@@ -2327,223 +2333,223 @@
         <v>131</v>
       </c>
       <c r="B124" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C124" t="n">
-        <v>0.32208320035144833</v>
+        <v>0.3985058446606471</v>
       </c>
       <c r="D124" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="B125" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C125" t="n">
-        <v>0.30970764546054863</v>
+        <v>0.3902222541548711</v>
       </c>
       <c r="D125" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>133</v>
+        <v>52</v>
       </c>
       <c r="B126" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C126" t="n">
-        <v>0.37966208728211054</v>
+        <v>0.3923034944103871</v>
       </c>
       <c r="D126" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C127" t="n">
-        <v>0.3979699876987751</v>
+        <v>0.2987263615155849</v>
       </c>
       <c r="D127" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="B128" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C128" t="n">
-        <v>0.3340889962145578</v>
+        <v>0.3231262658963662</v>
       </c>
       <c r="D128" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B129" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C129" t="n">
-        <v>0.3453402887458102</v>
+        <v>0.3083981974734053</v>
       </c>
       <c r="D129" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B130" t="s">
         <v>10</v>
       </c>
       <c r="C130" t="n">
-        <v>0.37023232824712726</v>
+        <v>0.3607013762065048</v>
       </c>
       <c r="D130" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B131" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C131" t="n">
-        <v>0.2736153602960227</v>
+        <v>0.01889362253402882</v>
       </c>
       <c r="D131" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B132" t="s">
         <v>10</v>
       </c>
       <c r="C132" t="n">
-        <v>0.3161669184150581</v>
+        <v>0.18053614627012338</v>
       </c>
       <c r="D132" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B133" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C133" t="n">
-        <v>0.24799123771051684</v>
+        <v>0.3954383254642092</v>
       </c>
       <c r="D133" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="B134" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C134" t="n">
-        <v>0.38692295539842</v>
+        <v>0.09306894171672817</v>
       </c>
       <c r="D134" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C135" t="n">
-        <v>0.22800464062382342</v>
+        <v>0.3840839467797417</v>
       </c>
       <c r="D135" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C136" t="n">
-        <v>0.39753694486923696</v>
+        <v>0.34902171629711637</v>
       </c>
       <c r="D136" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C137" t="n">
-        <v>0.2443168207760745</v>
+        <v>0.3901916757995627</v>
       </c>
       <c r="D137" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C138" t="n">
-        <v>0.3227197183652633</v>
+        <v>0.39321770092670827</v>
       </c>
       <c r="D138" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="B139" t="s">
         <v>5</v>
       </c>
       <c r="C139" t="n">
-        <v>0.38372251675728947</v>
+        <v>0.13531463834551302</v>
       </c>
       <c r="D139" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140">
@@ -2554,38 +2560,38 @@
         <v>10</v>
       </c>
       <c r="C140" t="n">
-        <v>0.2857144451806134</v>
+        <v>0.3328389360225405</v>
       </c>
       <c r="D140" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C141" t="n">
-        <v>0.3976438750684375</v>
+        <v>0.29748977689262995</v>
       </c>
       <c r="D141" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B142" t="s">
         <v>10</v>
       </c>
       <c r="C142" t="n">
-        <v>0.3838826112883563</v>
+        <v>0.35332916615451354</v>
       </c>
       <c r="D142" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143">
@@ -2593,13 +2599,13 @@
         <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C143" t="n">
-        <v>0.3885958780319866</v>
+        <v>0.3968131160113246</v>
       </c>
       <c r="D143" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
     </row>
     <row r="144">
@@ -2607,41 +2613,41 @@
         <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C144" t="n">
-        <v>0.23958594151700613</v>
+        <v>0.263258015121004</v>
       </c>
       <c r="D144" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>48</v>
+        <v>146</v>
       </c>
       <c r="B145" t="s">
         <v>10</v>
       </c>
       <c r="C145" t="n">
-        <v>0.2067229834447565</v>
+        <v>0.20273553598412983</v>
       </c>
       <c r="D145" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C146" t="n">
-        <v>0.39746341077488334</v>
+        <v>0.18164102826774078</v>
       </c>
       <c r="D146" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="147">
@@ -2649,13 +2655,13 @@
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C147" t="n">
-        <v>0.37103420123441366</v>
+        <v>0.04339837478972562</v>
       </c>
       <c r="D147" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="148">
@@ -2666,10 +2672,10 @@
         <v>5</v>
       </c>
       <c r="C148" t="n">
-        <v>0.3737802674008737</v>
+        <v>0.0925939437585529</v>
       </c>
       <c r="D148" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="149">
@@ -2677,13 +2683,13 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C149" t="n">
-        <v>0.3979182935798989</v>
+        <v>0.12105855028878561</v>
       </c>
       <c r="D149" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150">
@@ -2691,55 +2697,55 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C150" t="n">
-        <v>0.3031618774352718</v>
+        <v>0.23219152298094772</v>
       </c>
       <c r="D150" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="B151" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C151" t="n">
-        <v>0.22634113260693386</v>
+        <v>0.07034806629113849</v>
       </c>
       <c r="D151" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C152" t="n">
-        <v>0.3917762702589316</v>
+        <v>0.37775768569611856</v>
       </c>
       <c r="D152" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C153" t="n">
-        <v>0.3866718949828442</v>
+        <v>0.3859674850931559</v>
       </c>
       <c r="D153" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
     </row>
     <row r="154">
@@ -2747,391 +2753,391 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C154" t="n">
-        <v>0.1906118732119003</v>
+        <v>0.39884100897138797</v>
       </c>
       <c r="D154" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B155" t="s">
         <v>10</v>
       </c>
       <c r="C155" t="n">
-        <v>0.38755547477371777</v>
+        <v>0.21727060416514546</v>
       </c>
       <c r="D155" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C156" t="n">
-        <v>0.06172094937285739</v>
+        <v>0.336820852964416</v>
       </c>
       <c r="D156" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C157" t="n">
-        <v>0.052606664584758996</v>
+        <v>0.3173017999094758</v>
       </c>
       <c r="D157" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C158" t="n">
-        <v>0.23579486220019882</v>
+        <v>0.21553589442944687</v>
       </c>
       <c r="D158" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C159" t="n">
-        <v>0.39077914514837986</v>
+        <v>0.08092261638710281</v>
       </c>
       <c r="D159" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="B160" t="s">
         <v>10</v>
       </c>
       <c r="C160" t="n">
-        <v>0.3695226962670783</v>
+        <v>0.3652628138766605</v>
       </c>
       <c r="D160" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
       </c>
       <c r="C161" t="n">
-        <v>0.37527746383537003</v>
+        <v>0.3257928571113815</v>
       </c>
       <c r="D161" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C162" t="n">
-        <v>0.3825159409815373</v>
+        <v>0.021798765746537274</v>
       </c>
       <c r="D162" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B163" t="s">
         <v>10</v>
       </c>
       <c r="C163" t="n">
-        <v>0.3953338772612408</v>
+        <v>0.39372931702278297</v>
       </c>
       <c r="D163" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C164" t="n">
-        <v>0.15761636258407077</v>
+        <v>0.3123176250710959</v>
       </c>
       <c r="D164" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C165" t="n">
-        <v>0.3988193534146727</v>
+        <v>0.29172951651903817</v>
       </c>
       <c r="D165" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C166" t="n">
-        <v>0.33030736573320657</v>
+        <v>0.3357967539391835</v>
       </c>
       <c r="D166" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B167" t="s">
         <v>5</v>
       </c>
       <c r="C167" t="n">
-        <v>0.36817110912286477</v>
+        <v>0.3513222227128801</v>
       </c>
       <c r="D167" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C168" t="n">
-        <v>0.3985764812826302</v>
+        <v>0.3934704455141242</v>
       </c>
       <c r="D168" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C169" t="n">
-        <v>0.21688642977543254</v>
+        <v>0.25313911699163405</v>
       </c>
       <c r="D169" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C170" t="n">
-        <v>0.15415509696374408</v>
+        <v>0.3152878780159114</v>
       </c>
       <c r="D170" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B171" t="s">
         <v>10</v>
       </c>
       <c r="C171" t="n">
-        <v>0.3505871320143275</v>
+        <v>0.39765770051574956</v>
       </c>
       <c r="D171" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="B172" t="s">
         <v>10</v>
       </c>
       <c r="C172" t="n">
-        <v>0.3860850272589179</v>
+        <v>0.012526994592446147</v>
       </c>
       <c r="D172" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C173" t="n">
-        <v>0.3989420726070041</v>
+        <v>0.3942591012821005</v>
       </c>
       <c r="D173" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C174" t="n">
-        <v>0.266247959980625</v>
+        <v>0.3814277580563201</v>
       </c>
       <c r="D174" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C175" t="n">
-        <v>0.053967028268770305</v>
+        <v>0.33338897268292317</v>
       </c>
       <c r="D175" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B176" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C176" t="n">
-        <v>0.394953303746838</v>
+        <v>0.3971172754713456</v>
       </c>
       <c r="D176" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B177" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C177" t="n">
-        <v>0.38528417831985695</v>
+        <v>0.26146513951675004</v>
       </c>
       <c r="D177" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B178" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C178" t="n">
-        <v>0.2172316460266999</v>
+        <v>0.3472853899902795</v>
       </c>
       <c r="D178" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="B179" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C179" t="n">
-        <v>0.396728336774955</v>
+        <v>0.21209435852383468</v>
       </c>
       <c r="D179" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B180" t="s">
         <v>10</v>
       </c>
       <c r="C180" t="n">
-        <v>0.25582560639082746</v>
+        <v>0.33127630011631565</v>
       </c>
       <c r="D180" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C181" t="n">
-        <v>0.3365892951846078</v>
+        <v>0.3931687998271371</v>
       </c>
       <c r="D181" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added testProject csv and start of testing program
</commit_message>
<xml_diff>
--- a/Analysis120.xlsx
+++ b/Analysis120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="178">
   <si>
     <t>Research Activity</t>
   </si>
@@ -26,508 +26,526 @@
     <t>Percentage Distribution</t>
   </si>
   <si>
-    <t>playing rock music</t>
+    <t>singing middle-of-the-road songs</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
+    <t>0.67%</t>
+  </si>
+  <si>
+    <t>hunting raccoons</t>
+  </si>
+  <si>
+    <t>0.58%</t>
+  </si>
+  <si>
+    <t>singing Hipbop songs</t>
+  </si>
+  <si>
+    <t>promoting Buddhism</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>0.75%</t>
+  </si>
+  <si>
+    <t>running a propaganda machine</t>
+  </si>
+  <si>
+    <t>analyzing the sub-conscious</t>
+  </si>
+  <si>
+    <t>0.33%</t>
+  </si>
+  <si>
+    <t>promoting logical thinking</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>1.00%</t>
+  </si>
+  <si>
+    <t>terrorizing employees</t>
+  </si>
+  <si>
+    <t>interpreting evidence</t>
+  </si>
+  <si>
+    <t>cracking the whip</t>
+  </si>
+  <si>
+    <t>keeping a diary</t>
+  </si>
+  <si>
+    <t>playing tough guys</t>
+  </si>
+  <si>
+    <t>playing the violin</t>
+  </si>
+  <si>
     <t>0.17%</t>
   </si>
   <si>
+    <t>fighting for democracy</t>
+  </si>
+  <si>
+    <t>plagiarizing political speeches</t>
+  </si>
+  <si>
+    <t>racking up marriages</t>
+  </si>
+  <si>
+    <t>0.00%</t>
+  </si>
+  <si>
+    <t>winning heavyweight titles</t>
+  </si>
+  <si>
+    <t>peacocking in fancy clothes</t>
+  </si>
+  <si>
+    <t>running a crime family</t>
+  </si>
+  <si>
+    <t>0.25%</t>
+  </si>
+  <si>
+    <t>defending the weak</t>
+  </si>
+  <si>
+    <t>0.83%</t>
+  </si>
+  <si>
+    <t>running a kingdom</t>
+  </si>
+  <si>
+    <t>1.17%</t>
+  </si>
+  <si>
+    <t>ranting about liberals</t>
+  </si>
+  <si>
+    <t>solving mysteries</t>
+  </si>
+  <si>
+    <t>1.08%</t>
+  </si>
+  <si>
+    <t>engaging in hapless hijinks</t>
+  </si>
+  <si>
+    <t>hosting a late night chat show</t>
+  </si>
+  <si>
+    <t>0.50%</t>
+  </si>
+  <si>
+    <t>teaching philosophy</t>
+  </si>
+  <si>
+    <t>selling out</t>
+  </si>
+  <si>
+    <t>commanding Roman legions</t>
+  </si>
+  <si>
+    <t>selling consumer goods</t>
+  </si>
+  <si>
+    <t>moaning about women</t>
+  </si>
+  <si>
+    <t>1.33%</t>
+  </si>
+  <si>
+    <t>watching the sun rise</t>
+  </si>
+  <si>
+    <t>0.08%</t>
+  </si>
+  <si>
+    <t>beating menial staff</t>
+  </si>
+  <si>
+    <t>finding clues</t>
+  </si>
+  <si>
+    <t>developing political strategies</t>
+  </si>
+  <si>
+    <t>painting magazine covers</t>
+  </si>
+  <si>
+    <t>promoting conservative values</t>
+  </si>
+  <si>
+    <t>watching TV</t>
+  </si>
+  <si>
+    <t>doing stand-up</t>
+  </si>
+  <si>
+    <t>0.92%</t>
+  </si>
+  <si>
+    <t>composing classical music</t>
+  </si>
+  <si>
+    <t>painting colorful pictures</t>
+  </si>
+  <si>
+    <t>painting abstract pictures</t>
+  </si>
+  <si>
+    <t>singing torch songs</t>
+  </si>
+  <si>
+    <t>fighting with swords</t>
+  </si>
+  <si>
+    <t>playing the piano</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
+  </si>
+  <si>
+    <t>fighting for civil rights</t>
+  </si>
+  <si>
+    <t>getting a nose job</t>
+  </si>
+  <si>
+    <t>writing blues songs</t>
+  </si>
+  <si>
     <t>starring in Hollywood movies</t>
   </si>
   <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t>0.25%</t>
-  </si>
-  <si>
-    <t>moaning about men</t>
+    <t>flipping hamburgers</t>
+  </si>
+  <si>
+    <t>building rocket ships</t>
+  </si>
+  <si>
+    <t>doing raunchy stage acts</t>
+  </si>
+  <si>
+    <t>proving math theorems</t>
   </si>
   <si>
     <t>0.42%</t>
   </si>
   <si>
-    <t>making action movies</t>
-  </si>
-  <si>
-    <t>writing comedy</t>
-  </si>
-  <si>
-    <t>0.92%</t>
-  </si>
-  <si>
-    <t>running a multinational corporation</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>1.42%</t>
-  </si>
-  <si>
-    <t>singing torch songs</t>
-  </si>
-  <si>
-    <t>promoting greed</t>
-  </si>
-  <si>
-    <t>0.67%</t>
-  </si>
-  <si>
-    <t>handing out flowers</t>
-  </si>
-  <si>
-    <t>1.00%</t>
-  </si>
-  <si>
-    <t>playing basketball</t>
-  </si>
-  <si>
-    <t>0.58%</t>
-  </si>
-  <si>
-    <t>ranting about liberals</t>
-  </si>
-  <si>
-    <t>painting colorful pictures</t>
-  </si>
-  <si>
-    <t>0.50%</t>
-  </si>
-  <si>
-    <t>writing plays</t>
+    <t>seducing emperors</t>
+  </si>
+  <si>
+    <t>playing jazz saxophone</t>
+  </si>
+  <si>
+    <t>modeling DNA</t>
+  </si>
+  <si>
+    <t>writing modern fiction</t>
+  </si>
+  <si>
+    <t>solving crimes</t>
+  </si>
+  <si>
+    <t>starring in daytime soap operas</t>
+  </si>
+  <si>
+    <t>writing about social problems</t>
+  </si>
+  <si>
+    <t>divorcing husbands</t>
   </si>
   <si>
     <t>cross-dressing in women's clothes</t>
   </si>
   <si>
-    <t>promoting liberal values</t>
-  </si>
-  <si>
-    <t>commenting on social issues</t>
+    <t>giving noogies</t>
+  </si>
+  <si>
+    <t>pioneering new technologies</t>
+  </si>
+  <si>
+    <t>reading braille</t>
+  </si>
+  <si>
+    <t>playing the clarinet</t>
+  </si>
+  <si>
+    <t>writing folksy fiction</t>
+  </si>
+  <si>
+    <t>studying gorillas up close</t>
+  </si>
+  <si>
+    <t>causing mayhem</t>
+  </si>
+  <si>
+    <t>amassing wealth</t>
+  </si>
+  <si>
+    <t>looking for immortality</t>
+  </si>
+  <si>
+    <t>instigating rebellion</t>
+  </si>
+  <si>
+    <t>leading an exodus</t>
+  </si>
+  <si>
+    <t>running a criminal enterprise</t>
+  </si>
+  <si>
+    <t>promoting circus attractions</t>
+  </si>
+  <si>
+    <t>starring in romantic comedies</t>
+  </si>
+  <si>
+    <t>making subversive art</t>
+  </si>
+  <si>
+    <t>jumping on couches</t>
+  </si>
+  <si>
+    <t>breaking records</t>
+  </si>
+  <si>
+    <t>eluding the CIA</t>
+  </si>
+  <si>
+    <t>smoking cigarettes</t>
+  </si>
+  <si>
+    <t>directing Hollywood movies</t>
+  </si>
+  <si>
+    <t>drawing whimsical cartoons</t>
+  </si>
+  <si>
+    <t>directing bad movies</t>
+  </si>
+  <si>
+    <t>promoting movie violence</t>
+  </si>
+  <si>
+    <t>punishing criminals</t>
+  </si>
+  <si>
+    <t>playing ice hockey</t>
+  </si>
+  <si>
+    <t>selling comic books</t>
+  </si>
+  <si>
+    <t>giving speeches</t>
+  </si>
+  <si>
+    <t>promoting Heliocentrism</t>
+  </si>
+  <si>
+    <t>amassing ill-gotten wealth</t>
+  </si>
+  <si>
+    <t>losing control</t>
+  </si>
+  <si>
+    <t>collecting green Kryponite</t>
+  </si>
+  <si>
+    <t>teaching magic</t>
+  </si>
+  <si>
+    <t>running an empire</t>
+  </si>
+  <si>
+    <t>pushing dodgy operating systems</t>
+  </si>
+  <si>
+    <t>plotting with the enemy</t>
+  </si>
+  <si>
+    <t>pedalling engine-less cars</t>
+  </si>
+  <si>
+    <t>writing historical fiction</t>
+  </si>
+  <si>
+    <t>crushing dissent</t>
+  </si>
+  <si>
+    <t>talking in riddles</t>
+  </si>
+  <si>
+    <t>hunting aliens</t>
+  </si>
+  <si>
+    <t>1.25%</t>
+  </si>
+  <si>
+    <t>promoting the Dark Side</t>
+  </si>
+  <si>
+    <t>signing sports memorabilia</t>
+  </si>
+  <si>
+    <t>slapping soldiers</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
+  </si>
+  <si>
+    <t>running a business empire</t>
+  </si>
+  <si>
+    <t>winning tennis tournaments</t>
+  </si>
+  <si>
+    <t>writing serialized stories</t>
+  </si>
+  <si>
+    <t>spreading revolution</t>
+  </si>
+  <si>
+    <t>insulting minorities</t>
+  </si>
+  <si>
+    <t>foiling the schemes of evil villains</t>
+  </si>
+  <si>
+    <t>running a media empire</t>
+  </si>
+  <si>
+    <t>teaching philosophy to future leaders</t>
+  </si>
+  <si>
+    <t>standing up to bullies</t>
+  </si>
+  <si>
+    <t>mangling idioms</t>
+  </si>
+  <si>
+    <t>ruling over subjects</t>
+  </si>
+  <si>
+    <t>shopping for shoes</t>
+  </si>
+  <si>
+    <t>reporting for The Daily Planet</t>
+  </si>
+  <si>
+    <t>promoting Darwinism</t>
+  </si>
+  <si>
+    <t>promoting evolutionary theory</t>
+  </si>
+  <si>
+    <t>painting church ceilings</t>
+  </si>
+  <si>
+    <t>modeling clothes</t>
+  </si>
+  <si>
+    <t>delivering forehand slams</t>
+  </si>
+  <si>
+    <t>publishing soft pornography</t>
+  </si>
+  <si>
+    <t>cheating at poker</t>
+  </si>
+  <si>
+    <t>barking orders at subordinates</t>
+  </si>
+  <si>
+    <t>writing poetry</t>
+  </si>
+  <si>
+    <t>promoting Catholic values</t>
+  </si>
+  <si>
+    <t>building empires</t>
   </si>
   <si>
     <t>preparing for war</t>
   </si>
   <si>
-    <t>fighting the resistance</t>
-  </si>
-  <si>
-    <t>reporting for The Daily Planet</t>
-  </si>
-  <si>
-    <t>0.83%</t>
-  </si>
-  <si>
-    <t>promoting conservative values</t>
-  </si>
-  <si>
-    <t>0.33%</t>
-  </si>
-  <si>
-    <t>0.08%</t>
-  </si>
-  <si>
-    <t>punching out Nazis</t>
-  </si>
-  <si>
-    <t>0.00%</t>
-  </si>
-  <si>
-    <t>studying magic tricks</t>
-  </si>
-  <si>
-    <t>seducing emperors</t>
-  </si>
-  <si>
-    <t>throwing sex parties</t>
-  </si>
-  <si>
-    <t>selling consumer goods</t>
-  </si>
-  <si>
-    <t>seeking revenge</t>
-  </si>
-  <si>
-    <t>inventing electrical marvels</t>
-  </si>
-  <si>
-    <t>lecturing about climate change</t>
-  </si>
-  <si>
-    <t>pioneering new technologies</t>
-  </si>
-  <si>
-    <t>writing about sex</t>
-  </si>
-  <si>
-    <t>watching the sun rise</t>
-  </si>
-  <si>
-    <t>0.75%</t>
-  </si>
-  <si>
-    <t>writing TV comedies</t>
-  </si>
-  <si>
-    <t>promoting Eastern philosophy</t>
-  </si>
-  <si>
-    <t>composing classical music</t>
-  </si>
-  <si>
-    <t>promoting hair products</t>
-  </si>
-  <si>
-    <t>fighting for the rebel alliance</t>
-  </si>
-  <si>
-    <t>singing pop songs</t>
-  </si>
-  <si>
-    <t>testing scientific theories</t>
-  </si>
-  <si>
-    <t>chasing starlets</t>
-  </si>
-  <si>
-    <t>defending plaintiffs</t>
-  </si>
-  <si>
-    <t>playing soccer</t>
-  </si>
-  <si>
-    <t>designing clothes</t>
-  </si>
-  <si>
-    <t>carrying secret plans</t>
-  </si>
-  <si>
-    <t>starring in action movies</t>
-  </si>
-  <si>
-    <t>working for the forces of darkness</t>
-  </si>
-  <si>
-    <t>insulting minorities</t>
-  </si>
-  <si>
-    <t>killing people in ingenious ways</t>
-  </si>
-  <si>
-    <t>chasing criminals</t>
-  </si>
-  <si>
-    <t>1.08%</t>
-  </si>
-  <si>
-    <t>counting tooth picks</t>
-  </si>
-  <si>
-    <t>solving mysteries</t>
-  </si>
-  <si>
-    <t>1.33%</t>
-  </si>
-  <si>
-    <t>fighting for civil rights</t>
-  </si>
-  <si>
-    <t>singing to teenagers</t>
-  </si>
-  <si>
-    <t>piloting the Millenium Falcon</t>
-  </si>
-  <si>
-    <t>offering advice</t>
-  </si>
-  <si>
-    <t>finding clues</t>
-  </si>
-  <si>
-    <t>leading revolts</t>
-  </si>
-  <si>
-    <t>1.25%</t>
-  </si>
-  <si>
-    <t>writing modern fiction</t>
+    <t>winning boxing matches</t>
+  </si>
+  <si>
+    <t>clipping coupons</t>
+  </si>
+  <si>
+    <t>making prank calls</t>
+  </si>
+  <si>
+    <t>squandering money</t>
+  </si>
+  <si>
+    <t>avoiding growing old</t>
+  </si>
+  <si>
+    <t>raising new-age children</t>
+  </si>
+  <si>
+    <t>running restaurants</t>
+  </si>
+  <si>
+    <t>starring in comedies</t>
+  </si>
+  <si>
+    <t>opening new markets</t>
+  </si>
+  <si>
+    <t>executing morally appalling plans</t>
+  </si>
+  <si>
+    <t>telling bad jokes</t>
+  </si>
+  <si>
+    <t>teaching the next generation</t>
+  </si>
+  <si>
+    <t>singing country music</t>
+  </si>
+  <si>
+    <t>extracting confessions</t>
+  </si>
+  <si>
+    <t>piloting a spaceship</t>
+  </si>
+  <si>
+    <t>promoting tolerance</t>
+  </si>
+  <si>
+    <t>monetizing physical assets</t>
+  </si>
+  <si>
+    <t>promoting communism</t>
   </si>
   <si>
     <t>developing new technologies</t>
   </si>
   <si>
-    <t>flying into a rage</t>
-  </si>
-  <si>
-    <t>writing pop songs</t>
-  </si>
-  <si>
-    <t>running a business empire</t>
-  </si>
-  <si>
-    <t>making dumb comedies</t>
-  </si>
-  <si>
-    <t>writing about manly pursuits</t>
-  </si>
-  <si>
-    <t>running an empire</t>
-  </si>
-  <si>
-    <t>bodybuilding</t>
-  </si>
-  <si>
-    <t>representing criminals</t>
-  </si>
-  <si>
-    <t>smuggling contraband</t>
-  </si>
-  <si>
-    <t>1.17%</t>
-  </si>
-  <si>
-    <t>singing experimental songs</t>
-  </si>
-  <si>
-    <t>exploring foreign countries</t>
-  </si>
-  <si>
-    <t>doing stand-up</t>
-  </si>
-  <si>
-    <t>robbing banks</t>
-  </si>
-  <si>
-    <t>starring in reality TV shows</t>
-  </si>
-  <si>
-    <t>campaigning for world peace</t>
-  </si>
-  <si>
-    <t>recording pop songs</t>
-  </si>
-  <si>
-    <t>writing short stories</t>
-  </si>
-  <si>
-    <t>promoting communism</t>
-  </si>
-  <si>
-    <t>recruiting dissidents</t>
-  </si>
-  <si>
-    <t>peacocking in fancy clothes</t>
-  </si>
-  <si>
-    <t>opening new markets</t>
-  </si>
-  <si>
-    <t>driving under the influence</t>
-  </si>
-  <si>
-    <t>building houses for poor people</t>
-  </si>
-  <si>
-    <t>making trains run on time</t>
-  </si>
-  <si>
-    <t>developing operating systems</t>
-  </si>
-  <si>
-    <t>performing physical therapy</t>
-  </si>
-  <si>
-    <t>pulling dirty political tricks</t>
-  </si>
-  <si>
-    <t>pedalling furiously</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>frying crabby patties</t>
-  </si>
-  <si>
-    <t>promoting Fascism</t>
-  </si>
-  <si>
-    <t>looking for love</t>
-  </si>
-  <si>
-    <t>developing advertising campaigns</t>
-  </si>
-  <si>
-    <t>writing plays about the middle classes</t>
-  </si>
-  <si>
-    <t>eluding electronic ghosts</t>
-  </si>
-  <si>
-    <t>spouting movie trivia</t>
-  </si>
-  <si>
-    <t>studying science</t>
-  </si>
-  <si>
-    <t>preaching to presidents</t>
-  </si>
-  <si>
-    <t>promoting logical thinking</t>
-  </si>
-  <si>
-    <t>plotting election strategies</t>
-  </si>
-  <si>
-    <t>convicting criminals</t>
-  </si>
-  <si>
-    <t>promoting air travel</t>
-  </si>
-  <si>
-    <t>complaining about everything</t>
-  </si>
-  <si>
-    <t>assassinating presidents</t>
-  </si>
-  <si>
-    <t>preventing terrorism</t>
-  </si>
-  <si>
-    <t>podcasting about movies</t>
-  </si>
-  <si>
-    <t>running a technology company</t>
-  </si>
-  <si>
-    <t>writing in ledgers</t>
-  </si>
-  <si>
-    <t>suppressing violent urges</t>
-  </si>
-  <si>
-    <t>running a media empire</t>
-  </si>
-  <si>
-    <t>promoting capitalism</t>
-  </si>
-  <si>
-    <t>foiling the schemes of evil villains</t>
-  </si>
-  <si>
-    <t>wielding political power</t>
-  </si>
-  <si>
-    <t>teaching philosophy</t>
-  </si>
-  <si>
-    <t>painting realistic pictures</t>
-  </si>
-  <si>
-    <t>escaping from water tanks</t>
-  </si>
-  <si>
-    <t>avoiding paparazzi</t>
-  </si>
-  <si>
-    <t>preventing crime</t>
-  </si>
-  <si>
-    <t>chasing flappers</t>
-  </si>
-  <si>
-    <t>drawing whimsical cartoons</t>
-  </si>
-  <si>
-    <t>playing tough guys</t>
-  </si>
-  <si>
-    <t>writing mystery stories</t>
-  </si>
-  <si>
-    <t>smoking herb</t>
-  </si>
-  <si>
-    <t>moaning about women</t>
-  </si>
-  <si>
-    <t>killing murderers</t>
-  </si>
-  <si>
-    <t>singing country music</t>
-  </si>
-  <si>
-    <t>running a large metropolitan city</t>
-  </si>
-  <si>
-    <t>climbing social ladders</t>
-  </si>
-  <si>
-    <t>developing military strategies</t>
-  </si>
-  <si>
-    <t>fighting with swords</t>
-  </si>
-  <si>
-    <t>singing melancholy songs</t>
-  </si>
-  <si>
-    <t>running a criminal empire</t>
-  </si>
-  <si>
-    <t>building rocket ships</t>
-  </si>
-  <si>
-    <t>winning Michelin stars</t>
-  </si>
-  <si>
-    <t>writing poetry</t>
-  </si>
-  <si>
-    <t>instigating rebellion</t>
-  </si>
-  <si>
-    <t>inventing new technologies</t>
-  </si>
-  <si>
-    <t>racking up marriages</t>
-  </si>
-  <si>
-    <t>painting dark pictures</t>
-  </si>
-  <si>
-    <t>following the money</t>
-  </si>
-  <si>
-    <t>falling gracefully</t>
-  </si>
-  <si>
-    <t>offering medical opinions</t>
-  </si>
-  <si>
-    <t>leaking classified documents</t>
-  </si>
-  <si>
-    <t>making fantasy movies</t>
-  </si>
-  <si>
-    <t>investigating alien abductions</t>
-  </si>
-  <si>
-    <t>making escape plans</t>
-  </si>
-  <si>
-    <t>being a good neighbor</t>
-  </si>
-  <si>
-    <t>duelling acrobatically</t>
-  </si>
-  <si>
-    <t>building a search engine</t>
+    <t>singing on TV shows</t>
+  </si>
+  <si>
+    <t>fighting for justice</t>
+  </si>
+  <si>
+    <t>making bad movie choices</t>
+  </si>
+  <si>
+    <t>starring in cowboy movies</t>
   </si>
 </sst>
 </file>
@@ -585,7 +603,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="34.9609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="34.51171875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.69921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.85546875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="28.9375" customWidth="true" bestFit="true"/>
@@ -613,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>0.12365953745407593</v>
+        <v>0.3613589163797076</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -624,41 +642,41 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.3499527069389956</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.3081660877607913</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>0.36716977630315917</v>
+        <v>0.3839494192443864</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.38565677610462434</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.17221262028805595</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -669,38 +687,38 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2655117594509621</v>
+        <v>0.34721300939065286</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.30716189909850183</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.38845540188193356</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.35803247539940386</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.03288585961340481</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -708,1133 +726,1133 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>0.24978323433855135</v>
+        <v>0.3776089564525281</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3086112101385406</v>
+        <v>0.18415114438516134</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3461643239938675</v>
+        <v>0.3403137298580086</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.35624828191071906</v>
+      </c>
+      <c r="D12" t="s">
         <v>8</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.39132421848624854</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>0.25481152457306144</v>
+        <v>0.3426279069812939</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>0.30897974719167964</v>
+        <v>0.10288457976243759</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.38259560949729304</v>
+        <v>0.3614291468799365</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3901038070756383</v>
+        <v>0.3979502629320866</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C17" t="n">
-        <v>0.35457822594702904</v>
+        <v>0.03530062105299735</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>0.27788817386895714</v>
+        <v>0.3488570848264758</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.35352196312379774</v>
+        <v>0.37289321580780443</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" t="n">
-        <v>0.27811472405602516</v>
+        <v>0.07800562478211298</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2887532183039643</v>
+        <v>0.3623296090029224</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C22" t="n">
-        <v>0.12766579764148503</v>
+        <v>0.39838974907988034</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.39015153967339955</v>
+        <v>0.1928367141665386</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3892826310584495</v>
+        <v>0.39105843340250085</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01516138471618333</v>
+        <v>0.39022915934398616</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C26" t="n">
-        <v>0.38994686380694266</v>
+        <v>0.315316743965031</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>0.10526104554650073</v>
+        <v>0.1067224483380717</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>0.26093907813436523</v>
+        <v>0.38445574601827265</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.26504529794602527</v>
+      </c>
+      <c r="D29" t="s">
         <v>43</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.18584677865155758</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3981158216832802</v>
+        <v>0.3946283686132703</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2949012128340598</v>
+        <v>0.39738819456617386</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" t="n">
-        <v>0.25259837387002093</v>
+        <v>0.09067552524112603</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C33" t="n">
-        <v>0.37677821407813844</v>
+        <v>0.12457293593622759</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C34" t="n">
-        <v>0.23324768784803546</v>
+        <v>0.3144224233809197</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C35" t="n">
-        <v>0.3067249494379602</v>
+        <v>0.36705103293362207</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C36" t="n">
-        <v>0.3400192858795854</v>
+        <v>0.3181256234958282</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1969789147883943</v>
+        <v>0.08622435964840997</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C38" t="n">
-        <v>0.2364629732325973</v>
+        <v>0.24008076913782556</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1963999777565019</v>
+        <v>0.35338632579973517</v>
       </c>
       <c r="D39" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C40" t="n">
-        <v>0.11671925738023523</v>
+        <v>0.25210315861603555</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C41" t="n">
-        <v>0.36071431386035857</v>
+        <v>0.24305145579825574</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C42" t="n">
-        <v>0.3224424896438208</v>
+        <v>0.07376027455783786</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>0.19933285509828066</v>
+        <v>0.06188231309065065</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C44" t="n">
-        <v>0.08083283693597261</v>
+        <v>0.3985772609273141</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.3989387309035073</v>
+      </c>
+      <c r="D45" t="s">
         <v>8</v>
-      </c>
-      <c r="C45" t="n">
-        <v>0.34903379663558254</v>
-      </c>
-      <c r="D45" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>0.3989139469669982</v>
+        <v>0.3566589578628017</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C47" t="n">
-        <v>0.18810862037542894</v>
+        <v>0.03707414323572368</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C48" t="n">
-        <v>0.347740007437327</v>
+        <v>0.3646680845400972</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C49" t="n">
-        <v>0.3921122762843404</v>
+        <v>0.39727877865287015</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.3807742654742517</v>
+      </c>
+      <c r="D50" t="s">
         <v>8</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0.24421794261879945</v>
-      </c>
-      <c r="D50" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C51" t="n">
-        <v>0.36509615466475986</v>
+        <v>0.3247488672353838</v>
       </c>
       <c r="D51" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C52" t="n">
-        <v>0.13912601209466585</v>
+        <v>0.39751185237127984</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C53" t="n">
-        <v>0.152706692845559</v>
+        <v>0.3260412542703786</v>
       </c>
       <c r="D53" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C54" t="n">
-        <v>0.3939916535312771</v>
+        <v>0.268750897350418</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.2748630531424906</v>
+        <v>0.398911977080882</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C56" t="n">
-        <v>0.39876792017613866</v>
+        <v>0.3391176005316769</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C57" t="n">
-        <v>0.3663865152402292</v>
+        <v>0.2506176638371443</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C58" t="n">
-        <v>0.3986635675595113</v>
+        <v>0.2998732233592702</v>
       </c>
       <c r="D58" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C59" t="n">
-        <v>0.20571368375477841</v>
+        <v>0.17690630400131832</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C60" t="n">
-        <v>0.3548975411742942</v>
+        <v>0.39753606210216996</v>
       </c>
       <c r="D60" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C61" t="n">
-        <v>0.07476486079881246</v>
+        <v>0.07226610904327492</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C62" t="n">
-        <v>0.3520112472582488</v>
+        <v>0.3989228131435811</v>
       </c>
       <c r="D62" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3517973635248737</v>
+        <v>0.2603466623062578</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C64" t="n">
-        <v>0.07993519948598601</v>
+        <v>0.23145520032866346</v>
       </c>
       <c r="D64" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3962334563097132</v>
+        <v>0.12418401769245731</v>
       </c>
       <c r="D65" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
       </c>
       <c r="C66" t="n">
-        <v>0.39316243326708006</v>
+        <v>0.35002475047981807</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C67" t="n">
-        <v>0.2485267459194358</v>
+        <v>0.31940086193014827</v>
       </c>
       <c r="D67" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C68" t="n">
-        <v>0.17937095351282456</v>
+        <v>0.3425974706878172</v>
       </c>
       <c r="D68" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C69" t="n">
-        <v>0.003170425617031888</v>
+        <v>0.20089804761493774</v>
       </c>
       <c r="D69" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C70" t="n">
-        <v>0.13268138930978596</v>
+        <v>0.13742589712043377</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.23175585788654948</v>
+      </c>
+      <c r="D71" t="s">
         <v>8</v>
-      </c>
-      <c r="C71" t="n">
-        <v>0.3980529481707508</v>
-      </c>
-      <c r="D71" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C72" t="n">
-        <v>0.3380708317513376</v>
+        <v>0.05855943201433765</v>
       </c>
       <c r="D72" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C73" t="n">
-        <v>0.27693515359107357</v>
+        <v>0.2756679244465354</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C74" t="n">
-        <v>0.07046566766835163</v>
+        <v>0.31273478189992043</v>
       </c>
       <c r="D74" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C75" t="n">
-        <v>0.39838279261407145</v>
+        <v>0.238760310051521</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2660149345362879</v>
+        <v>0.36596207810020287</v>
       </c>
       <c r="D76" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C77" t="n">
-        <v>0.05861664668347628</v>
+        <v>0.39477016349489125</v>
       </c>
       <c r="D77" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C78" t="n">
-        <v>0.12755064387338266</v>
+        <v>0.3708144831545541</v>
       </c>
       <c r="D78" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C79" t="n">
-        <v>0.39883739011868574</v>
+        <v>0.36121770062254277</v>
       </c>
       <c r="D79" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C80" t="n">
-        <v>0.38120672526689475</v>
+        <v>0.23805826825612655</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C81" t="n">
-        <v>0.34338774094644026</v>
+        <v>0.22127837327754063</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C82" t="n">
-        <v>0.21774113798309477</v>
+        <v>0.2011175649739039</v>
       </c>
       <c r="D82" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3519214270761913</v>
+        <v>0.2107967759194273</v>
       </c>
       <c r="D83" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C84" t="n">
-        <v>0.04863864293838953</v>
+        <v>0.3875583060371585</v>
       </c>
       <c r="D84" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C85" t="n">
-        <v>0.3890763265647619</v>
+        <v>0.3430860245154223</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
       <c r="C86" t="n">
-        <v>0.3786112961307445</v>
+        <v>0.17039478226780858</v>
       </c>
       <c r="D86" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C87" t="n">
-        <v>0.3123177750385231</v>
+        <v>0.38263952739941737</v>
       </c>
       <c r="D87" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
       </c>
       <c r="C88" t="n">
-        <v>0.3529212435730347</v>
+        <v>0.37965107354129785</v>
       </c>
       <c r="D88" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.28575504630629966</v>
+      </c>
+      <c r="D89" t="s">
         <v>8</v>
-      </c>
-      <c r="C89" t="n">
-        <v>0.09227333916875784</v>
-      </c>
-      <c r="D89" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="90">
@@ -1842,13 +1860,13 @@
         <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C90" t="n">
-        <v>0.3985993715745561</v>
+        <v>0.39785092317071985</v>
       </c>
       <c r="D90" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91">
@@ -1856,13 +1874,13 @@
         <v>103</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C91" t="n">
-        <v>0.39747431251602994</v>
+        <v>0.12514707878851045</v>
       </c>
       <c r="D91" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92">
@@ -1870,13 +1888,13 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C92" t="n">
-        <v>0.2648311974789042</v>
+        <v>0.394656998790012</v>
       </c>
       <c r="D92" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93">
@@ -1884,13 +1902,13 @@
         <v>105</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C93" t="n">
-        <v>0.3579013315330324</v>
+        <v>0.24362579502706536</v>
       </c>
       <c r="D93" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="94">
@@ -1898,752 +1916,752 @@
         <v>106</v>
       </c>
       <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0.2789772013077871</v>
+      </c>
+      <c r="D94" t="s">
         <v>8</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0.3034873180936606</v>
-      </c>
-      <c r="D94" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95" t="n">
-        <v>0.36699602062983994</v>
+        <v>0.3629517546985584</v>
       </c>
       <c r="D95" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C96" t="n">
-        <v>0.25897535143439976</v>
+        <v>0.3448889838263782</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C97" t="n">
-        <v>0.39890444248500023</v>
+        <v>0.09906623854125886</v>
       </c>
       <c r="D97" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C98" t="n">
-        <v>0.09011786084235188</v>
+        <v>0.2941956073339778</v>
       </c>
       <c r="D98" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C99" t="n">
-        <v>0.38733628824757993</v>
+        <v>0.35219967125423646</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C100" t="n">
-        <v>0.36507778600493346</v>
+        <v>0.08612458387367171</v>
       </c>
       <c r="D100" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B101" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C101" t="n">
-        <v>0.29981050018305444</v>
+        <v>0.1377122159391883</v>
       </c>
       <c r="D101" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C102" t="n">
-        <v>0.30427328177379676</v>
+        <v>0.1967489679160405</v>
       </c>
       <c r="D102" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C103" t="n">
-        <v>0.16128021956448022</v>
+        <v>0.3972237656166417</v>
       </c>
       <c r="D103" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B104" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C104" t="n">
-        <v>0.37084387925311324</v>
+        <v>0.38192303557287155</v>
       </c>
       <c r="D104" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C105" t="n">
-        <v>0.3640868339126881</v>
+        <v>0.3015062129459662</v>
       </c>
       <c r="D105" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C106" t="n">
-        <v>0.26916621081657593</v>
+        <v>0.376098080544468</v>
       </c>
       <c r="D106" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B107" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C107" t="n">
-        <v>0.395038162282362</v>
+        <v>0.3982964678253852</v>
       </c>
       <c r="D107" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B108" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C108" t="n">
-        <v>0.22324043306376562</v>
+        <v>0.33339701344981626</v>
       </c>
       <c r="D108" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B109" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C109" t="n">
-        <v>0.3253705590312893</v>
+        <v>0.334893662450932</v>
       </c>
       <c r="D109" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="B110" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C110" t="n">
-        <v>0.38108727062800274</v>
+        <v>0.2745838911232384</v>
       </c>
       <c r="D110" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C111" t="n">
-        <v>0.2806994270505885</v>
+        <v>0.05549628012781462</v>
       </c>
       <c r="D111" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C112" t="n">
-        <v>0.108564306973777</v>
+        <v>0.10069450310579836</v>
       </c>
       <c r="D112" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B113" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C113" t="n">
-        <v>0.027871083217318182</v>
+        <v>0.3603883763506543</v>
       </c>
       <c r="D113" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1482178289084472</v>
+        <v>0.3317234489950848</v>
       </c>
       <c r="D114" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="B115" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C115" t="n">
-        <v>0.36760106756412353</v>
+        <v>0.3149172091135369</v>
       </c>
       <c r="D115" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B116" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C116" t="n">
-        <v>0.38235958636283246</v>
+        <v>0.13545678189515212</v>
       </c>
       <c r="D116" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C117" t="n">
-        <v>0.3837582364904139</v>
+        <v>0.24910498008352322</v>
       </c>
       <c r="D117" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
       </c>
       <c r="C118" t="n">
-        <v>0.3423453232763452</v>
+        <v>0.16812648282767953</v>
       </c>
       <c r="D118" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="B119" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1187445089662345</v>
+        <v>0.36899552981798034</v>
       </c>
       <c r="D119" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C120" t="n">
-        <v>0.3484502582847829</v>
+        <v>0.39397100631419657</v>
       </c>
       <c r="D120" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="B121" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C121" t="n">
-        <v>0.390289657973488</v>
+        <v>0.27852779026281343</v>
       </c>
       <c r="D121" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
       <c r="B122" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C122" t="n">
-        <v>0.3470059412680703</v>
+        <v>0.2100153883897429</v>
       </c>
       <c r="D122" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C123" t="n">
-        <v>0.25768560930183043</v>
+        <v>0.19255668515899327</v>
       </c>
       <c r="D123" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C124" t="n">
-        <v>0.11374854282001434</v>
+        <v>0.22805272241880192</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C125" t="n">
-        <v>0.3981047324961964</v>
+        <v>0.289350992296181</v>
       </c>
       <c r="D125" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C126" t="n">
-        <v>0.22769162070882282</v>
+        <v>0.39045809418870847</v>
       </c>
       <c r="D126" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
       </c>
       <c r="C127" t="n">
-        <v>0.2142189790153534</v>
+        <v>0.3945002870570656</v>
       </c>
       <c r="D127" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C128" t="n">
-        <v>0.3570974541261695</v>
+        <v>0.02113686968953285</v>
       </c>
       <c r="D128" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C129" t="n">
-        <v>0.3457319027252878</v>
+        <v>0.3179531380046384</v>
       </c>
       <c r="D129" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
       </c>
       <c r="C130" t="n">
-        <v>0.23188138640147207</v>
+        <v>0.3423114562419004</v>
       </c>
       <c r="D130" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" t="n">
+        <v>0.3412357592283956</v>
+      </c>
+      <c r="D131" t="s">
         <v>8</v>
-      </c>
-      <c r="C131" t="n">
-        <v>0.39278751721056177</v>
-      </c>
-      <c r="D131" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B132" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1455111829035462</v>
+        <v>0.11433231442140733</v>
       </c>
       <c r="D132" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B133" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C133" t="n">
-        <v>0.3929813928650322</v>
+        <v>0.3957218153611762</v>
       </c>
       <c r="D133" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
       </c>
       <c r="C134" t="n">
-        <v>0.23090430459012123</v>
+        <v>0.38095245230679564</v>
       </c>
       <c r="D134" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C135" t="n">
-        <v>0.39398740776299956</v>
+        <v>0.2228970882669236</v>
       </c>
       <c r="D135" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C136" t="n">
-        <v>0.3024945657620344</v>
+        <v>0.36104309603866475</v>
       </c>
       <c r="D136" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C137" t="n">
-        <v>0.36677987510853155</v>
+        <v>0.2872251203964793</v>
       </c>
       <c r="D137" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B138" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C138" t="n">
-        <v>0.3485315760211907</v>
+        <v>0.14527820799870544</v>
       </c>
       <c r="D138" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C139" t="n">
-        <v>0.35109814734970607</v>
+        <v>0.2417605646262015</v>
       </c>
       <c r="D139" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B140" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1840503744692187</v>
+        <v>0.39510893553128873</v>
       </c>
       <c r="D140" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="B141" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C141" t="n">
-        <v>0.048367741734063045</v>
+        <v>0.10108442510608799</v>
       </c>
       <c r="D141" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C142" t="n">
-        <v>0.3917997703652274</v>
+        <v>0.1961352070106947</v>
       </c>
       <c r="D142" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B143" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C143" t="n">
-        <v>0.04540213517876337</v>
+        <v>0.36069608086515187</v>
       </c>
       <c r="D143" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B144" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C144" t="n">
-        <v>0.37696088836088176</v>
+        <v>0.307162156980086</v>
       </c>
       <c r="D144" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C145" t="n">
-        <v>0.3611795885493117</v>
+        <v>0.37339224771437424</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B146" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1337866014742023</v>
+        <v>0.2925337053249385</v>
       </c>
       <c r="D146" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="B147" t="s">
         <v>5</v>
       </c>
       <c r="C147" t="n">
-        <v>0.3203917348152778</v>
+        <v>0.07660823463199788</v>
       </c>
       <c r="D147" t="s">
         <v>51</v>
@@ -2651,478 +2669,478 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B148" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C148" t="n">
-        <v>0.25034373018886763</v>
+        <v>0.3927252820336489</v>
       </c>
       <c r="D148" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C149" t="n">
-        <v>0.28781589526339313</v>
+        <v>0.06843389232029021</v>
       </c>
       <c r="D149" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B150" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C150" t="n">
-        <v>0.3928487164262549</v>
+        <v>0.37801579852139844</v>
       </c>
       <c r="D150" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B151" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C151" t="n">
-        <v>0.359334822151169</v>
+        <v>0.2952408888377462</v>
       </c>
       <c r="D151" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B152" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C152" t="n">
-        <v>0.38305107487702605</v>
+        <v>0.34645052491684813</v>
       </c>
       <c r="D152" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="B153" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C153" t="n">
-        <v>0.30067560370898144</v>
+        <v>0.20580904305607237</v>
       </c>
       <c r="D153" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="B154" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C154" t="n">
-        <v>0.2402827142099178</v>
+        <v>0.32301313447355606</v>
       </c>
       <c r="D154" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C155" t="n">
-        <v>0.35907520556829725</v>
+        <v>0.3876203109655054</v>
       </c>
       <c r="D155" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="B156" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C156" t="n">
-        <v>0.13868713681582848</v>
+        <v>0.3981283347712536</v>
       </c>
       <c r="D156" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B157" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C157" t="n">
-        <v>0.38170717411526084</v>
+        <v>0.3708668599494366</v>
       </c>
       <c r="D157" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B158" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C158" t="n">
-        <v>0.12178851855999381</v>
+        <v>0.23099110251016838</v>
       </c>
       <c r="D158" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="B159" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C159" t="n">
-        <v>0.39048833574447833</v>
+        <v>0.01739592821964612</v>
       </c>
       <c r="D159" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C160" t="n">
-        <v>0.0765309501823811</v>
+        <v>0.08034153914311831</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="B161" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C161" t="n">
-        <v>0.37615357518452974</v>
+        <v>0.19413280509945033</v>
       </c>
       <c r="D161" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="B162" t="s">
         <v>5</v>
       </c>
       <c r="C162" t="n">
-        <v>0.1410652520613998</v>
+        <v>0.38930279274814533</v>
       </c>
       <c r="D162" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B163" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C163" t="n">
-        <v>0.1024251835908396</v>
+        <v>0.35489954217358616</v>
       </c>
       <c r="D163" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C164" t="n">
-        <v>0.38468272501345163</v>
+        <v>0.3974159719489769</v>
       </c>
       <c r="D164" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C165" t="n">
-        <v>0.15841345977590288</v>
+        <v>0.17057401383019294</v>
       </c>
       <c r="D165" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C166" t="n">
-        <v>0.3957061533717947</v>
+        <v>0.3985552999228185</v>
       </c>
       <c r="D166" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C167" t="n">
-        <v>0.3408823498110449</v>
+        <v>0.38655060586700934</v>
       </c>
       <c r="D167" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>160</v>
+        <v>63</v>
       </c>
       <c r="B168" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C168" t="n">
-        <v>0.1419411656589489</v>
+        <v>0.36673035957293304</v>
       </c>
       <c r="D168" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C169" t="n">
-        <v>0.33732960786966026</v>
+        <v>0.3221259966002381</v>
       </c>
       <c r="D169" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C170" t="n">
-        <v>0.08913940893535027</v>
+        <v>0.2901821713314167</v>
       </c>
       <c r="D170" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>163</v>
+        <v>63</v>
       </c>
       <c r="B171" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C171" t="n">
-        <v>0.35266867189117745</v>
+        <v>0.3986338015294776</v>
       </c>
       <c r="D171" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="B172" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C172" t="n">
-        <v>0.13079041473158398</v>
+        <v>0.35370211041069377</v>
       </c>
       <c r="D172" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B173" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C173" t="n">
-        <v>0.15833022759860066</v>
+        <v>0.007309782343765086</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B174" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C174" t="n">
-        <v>0.34109581055458865</v>
+        <v>0.35550512480586377</v>
       </c>
       <c r="D174" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B175" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C175" t="n">
-        <v>0.3938848377602154</v>
+        <v>0.21052716003408145</v>
       </c>
       <c r="D175" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B176" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C176" t="n">
-        <v>0.024375451233784803</v>
+        <v>0.17526814575184482</v>
       </c>
       <c r="D176" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="B177" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C177" t="n">
-        <v>0.2748343890926546</v>
+        <v>0.365761970804521</v>
       </c>
       <c r="D177" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B178" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C178" t="n">
-        <v>0.37749041399118927</v>
+        <v>0.20620789085668426</v>
       </c>
       <c r="D178" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B179" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C179" t="n">
-        <v>0.38217542186347697</v>
+        <v>0.3988497959388734</v>
       </c>
       <c r="D179" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B180" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C180" t="n">
-        <v>0.221166757240653</v>
+        <v>0.26387867239532675</v>
       </c>
       <c r="D180" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>55</v>
+        <v>177</v>
       </c>
       <c r="B181" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C181" t="n">
-        <v>0.2659021714911606</v>
+        <v>0.36438569934092374</v>
       </c>
       <c r="D181" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>